<commit_message>
Updated permissions for Joinder Upload.
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$965</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$968</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="87">
   <si>
     <t>User</t>
   </si>
@@ -458,7 +458,151 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -697,10 +841,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N965"/>
+  <dimension ref="A1:N968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,7 +915,7 @@
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
-        <f t="shared" ref="A3:A66" si="0">ROW() - 1</f>
+        <f t="shared" ref="A3:A67" si="0">ROW() - 1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1679,11 +1823,11 @@
       <c r="C34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>39</v>
+      <c r="D34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>10</v>
@@ -1702,58 +1846,58 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>7</v>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="F36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
@@ -1767,13 +1911,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -1796,7 +1940,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>9</v>
@@ -1822,16 +1966,16 @@
         <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1854,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>17</v>
@@ -1883,7 +2027,7 @@
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>17</v>
@@ -1912,7 +2056,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>17</v>
@@ -1941,13 +2085,13 @@
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -1966,17 +2110,17 @@
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1999,7 +2143,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>17</v>
@@ -2024,11 +2168,11 @@
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>17</v>
@@ -2051,19 +2195,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2083,13 +2227,13 @@
         <v>44</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>10</v>
@@ -2115,10 +2259,10 @@
         <v>11</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>10</v>
@@ -2143,8 +2287,8 @@
       <c r="C50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="10" t="s">
-        <v>14</v>
+      <c r="D50" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>13</v>
@@ -2166,17 +2310,17 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>10</v>
@@ -2195,14 +2339,14 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>15</v>
+      <c r="D52" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>8</v>
@@ -2231,9 +2375,9 @@
         <v>11</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="2" t="s">
@@ -2257,16 +2401,16 @@
         <v>44</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -2286,13 +2430,13 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>19</v>
@@ -2318,7 +2462,7 @@
         <v>11</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>17</v>
@@ -2347,7 +2491,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>17</v>
@@ -2376,7 +2520,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>17</v>
@@ -2405,7 +2549,7 @@
         <v>11</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>17</v>
@@ -2434,7 +2578,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>17</v>
@@ -2463,7 +2607,7 @@
         <v>11</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>17</v>
@@ -2489,16 +2633,16 @@
         <v>44</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -2521,7 +2665,7 @@
         <v>7</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>9</v>
@@ -2547,16 +2691,16 @@
         <v>44</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -2575,11 +2719,11 @@
       <c r="B65" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>26</v>
@@ -2608,7 +2752,7 @@
         <v>11</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>26</v>
@@ -2627,23 +2771,23 @@
     </row>
     <row r="67" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
-        <f t="shared" ref="A67:A131" si="1">ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>7</v>
+      <c r="C67" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -2656,7 +2800,7 @@
     </row>
     <row r="68" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A68:A134" si="1">ROW() - 1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -2665,11 +2809,11 @@
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="10" t="s">
-        <v>86</v>
+      <c r="D68" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>10</v>
@@ -2692,13 +2836,13 @@
         <v>44</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>10</v>
@@ -2724,10 +2868,10 @@
         <v>11</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>10</v>
@@ -2753,13 +2897,13 @@
         <v>11</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2782,13 +2926,13 @@
         <v>11</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -2808,16 +2952,16 @@
         <v>44</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -2836,14 +2980,14 @@
       <c r="B74" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>11</v>
+      <c r="C74" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>19</v>
@@ -2869,7 +3013,7 @@
         <v>11</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>45</v>
@@ -2898,7 +3042,7 @@
         <v>11</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>45</v>
@@ -2924,13 +3068,13 @@
         <v>44</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>19</v>
@@ -2953,16 +3097,16 @@
         <v>44</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -2985,10 +3129,10 @@
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>10</v>
@@ -3014,13 +3158,13 @@
         <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3043,13 +3187,13 @@
         <v>11</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -3072,10 +3216,10 @@
         <v>11</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>10</v>
@@ -3101,12 +3245,14 @@
         <v>11</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F83" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -3122,16 +3268,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>10</v>
@@ -3151,19 +3297,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -3183,16 +3329,16 @@
         <v>49</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -3212,13 +3358,13 @@
         <v>49</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>19</v>
@@ -3244,7 +3390,7 @@
         <v>11</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>17</v>
@@ -3273,7 +3419,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>17</v>
@@ -3302,7 +3448,7 @@
         <v>11</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>17</v>
@@ -3331,7 +3477,7 @@
         <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>17</v>
@@ -3360,7 +3506,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>17</v>
@@ -3386,13 +3532,13 @@
         <v>49</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>19</v>
@@ -3418,10 +3564,10 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>19</v>
@@ -3444,13 +3590,13 @@
         <v>49</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>19</v>
@@ -3476,7 +3622,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>51</v>
@@ -3501,11 +3647,11 @@
       <c r="B97" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>51</v>
@@ -3530,11 +3676,11 @@
       <c r="B98" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>51</v>
@@ -3559,17 +3705,17 @@
       <c r="B99" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>7</v>
+      <c r="C99" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -3588,17 +3734,17 @@
       <c r="B100" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>7</v>
+      <c r="C100" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -3617,17 +3763,17 @@
       <c r="B101" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>11</v>
+      <c r="C101" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -3646,17 +3792,17 @@
       <c r="B102" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C102" s="5" t="s">
-        <v>11</v>
+      <c r="C102" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -3679,7 +3825,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>26</v>
@@ -3705,16 +3851,16 @@
         <v>49</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
@@ -3737,13 +3883,13 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -3763,13 +3909,13 @@
         <v>49</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>10</v>
@@ -3795,13 +3941,13 @@
         <v>11</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -3824,13 +3970,13 @@
         <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -3853,13 +3999,13 @@
         <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -3882,7 +4028,7 @@
         <v>11</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>57</v>
@@ -3911,13 +4057,13 @@
         <v>11</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
@@ -3940,13 +4086,13 @@
         <v>11</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
@@ -3969,13 +4115,13 @@
         <v>11</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -3986,34 +4132,34 @@
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
     </row>
-    <row r="114" spans="1:14" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="20">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="B114" s="13" t="s">
+      <c r="B114" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C114" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E114" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F114" s="13" t="s">
+      <c r="C114" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G114" s="13"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-      <c r="J114" s="13"/>
-      <c r="K114" s="13"/>
-      <c r="L114" s="13"/>
-      <c r="M114" s="13"/>
-      <c r="N114" s="13"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
     </row>
     <row r="115" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="20">
@@ -4024,16 +4170,16 @@
         <v>49</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
@@ -4044,34 +4190,34 @@
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
     </row>
-    <row r="116" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="20">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C116" s="5" t="s">
+      <c r="C116" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E116" s="2" t="s">
+      <c r="D116" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E116" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2"/>
-      <c r="N116" s="2"/>
+      <c r="F116" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13"/>
+      <c r="L116" s="13"/>
+      <c r="M116" s="13"/>
+      <c r="N116" s="13"/>
     </row>
     <row r="117" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="20">
@@ -4085,7 +4231,7 @@
         <v>7</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>9</v>
@@ -4114,7 +4260,7 @@
         <v>7</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>9</v>
@@ -4143,7 +4289,7 @@
         <v>7</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>9</v>
@@ -4165,58 +4311,58 @@
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D120" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E120" s="3" t="s">
+      <c r="D120" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E120" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F120" s="6" t="s">
+      <c r="F120" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="3"/>
-      <c r="L120" s="3"/>
-      <c r="M120" s="3"/>
-      <c r="N120" s="3"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2"/>
     </row>
     <row r="121" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="20">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D121" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E121" s="3" t="s">
+      <c r="D121" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E121" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F121" s="6" t="s">
+      <c r="F121" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3"/>
-      <c r="J121" s="3"/>
-      <c r="K121" s="3"/>
-      <c r="L121" s="3"/>
-      <c r="M121" s="3"/>
-      <c r="N121" s="3"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2"/>
     </row>
     <row r="122" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="20">
@@ -4227,13 +4373,13 @@
         <v>49</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E122" s="10" t="s">
-        <v>86</v>
+        <v>67</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F122" s="6" t="s">
         <v>19</v>
@@ -4252,20 +4398,20 @@
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C123" s="2" t="s">
+      <c r="B123" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E123" s="2" t="s">
+      <c r="D123" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F123" s="2" t="s">
-        <v>10</v>
+      <c r="F123" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
@@ -4281,19 +4427,19 @@
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F124" s="2" t="s">
+      <c r="B124" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F124" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G124" s="3"/>
@@ -4311,28 +4457,28 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C125" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C125" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D125" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>17</v>
+      <c r="D125" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E125" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G125" s="3"/>
-      <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
-      <c r="J125" s="3"/>
-      <c r="K125" s="3"/>
-      <c r="L125" s="3"/>
-      <c r="M125" s="3"/>
-      <c r="N125" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2"/>
+      <c r="M125" s="2"/>
+      <c r="N125" s="2"/>
     </row>
     <row r="126" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="20">
@@ -4343,16 +4489,16 @@
         <v>70</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D126" s="10" t="s">
-        <v>84</v>
+        <v>7</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
@@ -4372,13 +4518,13 @@
         <v>70</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>19</v>
@@ -4404,7 +4550,7 @@
         <v>11</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>17</v>
@@ -4432,8 +4578,8 @@
       <c r="C129" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>22</v>
+      <c r="D129" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>17</v>
@@ -4462,7 +4608,7 @@
         <v>11</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>17</v>
@@ -4491,7 +4637,7 @@
         <v>11</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>17</v>
@@ -4510,20 +4656,20 @@
     </row>
     <row r="132" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="20">
-        <f t="shared" ref="A132:A159" si="2">ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>19</v>
@@ -4539,7 +4685,7 @@
     </row>
     <row r="133" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
@@ -4549,10 +4695,10 @@
         <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>19</v>
@@ -4568,7 +4714,7 @@
     </row>
     <row r="134" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
@@ -4578,10 +4724,10 @@
         <v>11</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>19</v>
@@ -4597,20 +4743,20 @@
     </row>
     <row r="135" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A135:A163" si="2">ROW() - 1</f>
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>19</v>
@@ -4632,11 +4778,11 @@
       <c r="B136" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C136" s="5" t="s">
+      <c r="C136" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>51</v>
@@ -4661,11 +4807,11 @@
       <c r="B137" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C137" s="5" t="s">
+      <c r="C137" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>51</v>
@@ -4691,16 +4837,16 @@
         <v>70</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
@@ -4719,17 +4865,17 @@
       <c r="B139" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>7</v>
+      <c r="C139" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
@@ -4752,10 +4898,10 @@
         <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>19</v>
@@ -4777,17 +4923,17 @@
       <c r="B141" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C141" s="5" t="s">
-        <v>11</v>
+      <c r="C141" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
@@ -4806,17 +4952,17 @@
       <c r="B142" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C142" s="5" t="s">
-        <v>11</v>
+      <c r="C142" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
@@ -4836,16 +4982,16 @@
         <v>70</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
@@ -4868,13 +5014,13 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
@@ -4897,13 +5043,13 @@
         <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
@@ -4923,16 +5069,16 @@
         <v>70</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
@@ -4955,22 +5101,22 @@
         <v>11</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
-      <c r="L147" s="2"/>
-      <c r="M147" s="2"/>
-      <c r="N147" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="3"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
     </row>
     <row r="148" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="20">
@@ -4984,7 +5130,7 @@
         <v>11</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>57</v>
@@ -4992,14 +5138,14 @@
       <c r="F148" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-      <c r="L148" s="2"/>
-      <c r="M148" s="2"/>
-      <c r="N148" s="2"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
     </row>
     <row r="149" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="20">
@@ -5013,7 +5159,7 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>57</v>
@@ -5021,14 +5167,14 @@
       <c r="F149" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
-      <c r="J149" s="2"/>
-      <c r="K149" s="2"/>
-      <c r="L149" s="2"/>
-      <c r="M149" s="2"/>
-      <c r="N149" s="2"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
     </row>
     <row r="150" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="20">
@@ -5042,7 +5188,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>57</v>
@@ -5071,7 +5217,7 @@
         <v>11</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>57</v>
@@ -5100,13 +5246,13 @@
         <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
@@ -5125,17 +5271,17 @@
       <c r="B153" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>7</v>
+      <c r="C153" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
@@ -5155,16 +5301,16 @@
         <v>70</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D154" s="10" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
@@ -5184,16 +5330,16 @@
         <v>70</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
@@ -5215,14 +5361,14 @@
       <c r="C156" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D156" s="10" t="s">
-        <v>67</v>
+      <c r="D156" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
@@ -5244,8 +5390,8 @@
       <c r="C157" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D157" s="3" t="s">
-        <v>68</v>
+      <c r="D157" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>9</v>
@@ -5274,7 +5420,7 @@
         <v>7</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>9</v>
@@ -5299,17 +5445,17 @@
       <c r="B159" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C159" s="5" t="s">
-        <v>11</v>
+      <c r="C159" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
@@ -5321,12 +5467,25 @@
       <c r="N159" s="2"/>
     </row>
     <row r="160" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A160" s="20"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="5"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
+      <c r="A160" s="20">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
@@ -5337,12 +5496,25 @@
       <c r="N160" s="2"/>
     </row>
     <row r="161" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A161" s="20"/>
-      <c r="B161" s="2"/>
-      <c r="C161" s="5"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
+      <c r="A161" s="20">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G161" s="2"/>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -5353,12 +5525,25 @@
       <c r="N161" s="2"/>
     </row>
     <row r="162" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A162" s="20"/>
-      <c r="B162" s="2"/>
-      <c r="C162" s="5"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
+      <c r="A162" s="20">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -5369,12 +5554,25 @@
       <c r="N162" s="2"/>
     </row>
     <row r="163" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A163" s="20"/>
-      <c r="B163" s="2"/>
-      <c r="C163" s="5"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
+      <c r="A163" s="20">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E163" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G163" s="2"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
@@ -5403,7 +5601,7 @@
     <row r="165" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="20"/>
       <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
+      <c r="C165" s="5"/>
       <c r="D165" s="3"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
@@ -5451,7 +5649,7 @@
     <row r="168" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="20"/>
       <c r="B168" s="2"/>
-      <c r="C168" s="5"/>
+      <c r="C168" s="2"/>
       <c r="D168" s="3"/>
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
@@ -5483,8 +5681,8 @@
     <row r="170" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-      <c r="D170" s="2"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="3"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
@@ -5499,8 +5697,8 @@
     <row r="171" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
-      <c r="D171" s="2"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="3"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
@@ -5515,8 +5713,8 @@
     <row r="172" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="20"/>
       <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
-      <c r="D172" s="2"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="3"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
@@ -18216,6 +18414,54 @@
       <c r="M965" s="2"/>
       <c r="N965" s="2"/>
     </row>
+    <row r="966" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A966" s="20"/>
+      <c r="B966" s="2"/>
+      <c r="C966" s="2"/>
+      <c r="D966" s="2"/>
+      <c r="E966" s="2"/>
+      <c r="F966" s="2"/>
+      <c r="G966" s="2"/>
+      <c r="H966" s="2"/>
+      <c r="I966" s="2"/>
+      <c r="J966" s="2"/>
+      <c r="K966" s="2"/>
+      <c r="L966" s="2"/>
+      <c r="M966" s="2"/>
+      <c r="N966" s="2"/>
+    </row>
+    <row r="967" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A967" s="20"/>
+      <c r="B967" s="2"/>
+      <c r="C967" s="2"/>
+      <c r="D967" s="2"/>
+      <c r="E967" s="2"/>
+      <c r="F967" s="2"/>
+      <c r="G967" s="2"/>
+      <c r="H967" s="2"/>
+      <c r="I967" s="2"/>
+      <c r="J967" s="2"/>
+      <c r="K967" s="2"/>
+      <c r="L967" s="2"/>
+      <c r="M967" s="2"/>
+      <c r="N967" s="2"/>
+    </row>
+    <row r="968" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A968" s="20"/>
+      <c r="B968" s="2"/>
+      <c r="C968" s="2"/>
+      <c r="D968" s="2"/>
+      <c r="E968" s="2"/>
+      <c r="F968" s="2"/>
+      <c r="G968" s="2"/>
+      <c r="H968" s="2"/>
+      <c r="I968" s="2"/>
+      <c r="J968" s="2"/>
+      <c r="K968" s="2"/>
+      <c r="L968" s="2"/>
+      <c r="M968" s="2"/>
+      <c r="N968" s="2"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
@@ -18223,15 +18469,48 @@
       <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F1:F965">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
+  <conditionalFormatting sqref="F1:F83 F85:F124 F126:F162 F164:F968">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH(("No"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Write">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="Write">
       <formula>NOT(ISERROR(SEARCH(("Write"),(F1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F84))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F84))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F84))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F125">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F125))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F125))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F125))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F163">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F163))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F163))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F163))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18283,7 +18562,7 @@
   <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add per lits permissions.
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$964</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$967</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="90">
   <si>
     <t>User</t>
   </si>
@@ -301,6 +301,15 @@
   <si>
     <t>document-repository-comp</t>
   </si>
+  <si>
+    <t>per-list-comp</t>
+  </si>
+  <si>
+    <t>human-per-list-comp</t>
+  </si>
+  <si>
+    <t>playbooks-comp</t>
+  </si>
 </sst>
 </file>
 
@@ -458,7 +467,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -769,18 +898,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N964"/>
+  <dimension ref="A1:N967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.44140625" style="21" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="37.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -843,7 +972,7 @@
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
-        <f t="shared" ref="A3:A66" si="0">ROW() - 1</f>
+        <f t="shared" ref="A3:A67" si="0">ROW() - 1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1774,58 +1903,58 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="4" t="s">
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="F36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
@@ -1839,13 +1968,13 @@
         <v>7</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -1868,7 +1997,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>9</v>
@@ -1894,16 +2023,16 @@
         <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1926,7 +2055,7 @@
         <v>11</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>17</v>
@@ -1955,7 +2084,7 @@
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>17</v>
@@ -1984,7 +2113,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>17</v>
@@ -2013,13 +2142,13 @@
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2038,17 +2167,17 @@
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2071,7 +2200,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>17</v>
@@ -2096,11 +2225,11 @@
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>17</v>
@@ -2123,19 +2252,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2155,13 +2284,13 @@
         <v>44</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>10</v>
@@ -2187,10 +2316,10 @@
         <v>11</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>10</v>
@@ -2215,8 +2344,8 @@
       <c r="C50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="10" t="s">
-        <v>14</v>
+      <c r="D50" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>13</v>
@@ -2238,17 +2367,17 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>10</v>
@@ -2267,14 +2396,14 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>15</v>
+      <c r="D52" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>8</v>
@@ -2303,9 +2432,9 @@
         <v>11</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="2" t="s">
@@ -2329,16 +2458,16 @@
         <v>44</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -2358,13 +2487,13 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>19</v>
@@ -2390,7 +2519,7 @@
         <v>11</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>17</v>
@@ -2419,7 +2548,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>17</v>
@@ -2448,7 +2577,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>17</v>
@@ -2477,7 +2606,7 @@
         <v>11</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>17</v>
@@ -2506,7 +2635,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>17</v>
@@ -2535,7 +2664,7 @@
         <v>11</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>17</v>
@@ -2561,16 +2690,16 @@
         <v>44</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -2593,7 +2722,7 @@
         <v>7</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>9</v>
@@ -2619,16 +2748,16 @@
         <v>44</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -2647,11 +2776,11 @@
       <c r="B65" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>26</v>
@@ -2680,7 +2809,7 @@
         <v>11</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>26</v>
@@ -2699,23 +2828,23 @@
     </row>
     <row r="67" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
-        <f t="shared" ref="A67:A130" si="1">ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>7</v>
+      <c r="C67" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -2728,20 +2857,20 @@
     </row>
     <row r="68" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A68:A133" si="1">ROW() - 1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>10</v>
@@ -2767,13 +2896,13 @@
         <v>11</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -2796,13 +2925,13 @@
         <v>11</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2822,16 +2951,16 @@
         <v>44</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2850,14 +2979,14 @@
       <c r="B72" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>11</v>
+      <c r="C72" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>19</v>
@@ -2883,7 +3012,7 @@
         <v>11</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>45</v>
@@ -2912,7 +3041,7 @@
         <v>11</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>45</v>
@@ -2938,13 +3067,13 @@
         <v>44</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>19</v>
@@ -2967,16 +3096,16 @@
         <v>44</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -2999,10 +3128,10 @@
         <v>11</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>10</v>
@@ -3028,13 +3157,13 @@
         <v>11</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -3057,13 +3186,13 @@
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3086,10 +3215,10 @@
         <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>10</v>
@@ -3114,11 +3243,11 @@
       <c r="C81" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>33</v>
+      <c r="D81" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>10</v>
@@ -3143,11 +3272,11 @@
       <c r="C82" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>35</v>
+      <c r="D82" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>10</v>
@@ -3173,10 +3302,10 @@
         <v>11</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>10</v>
@@ -3196,16 +3325,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>10</v>
@@ -3224,20 +3353,20 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>9</v>
+      <c r="B85" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -3257,16 +3386,16 @@
         <v>49</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -3286,13 +3415,13 @@
         <v>49</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>19</v>
@@ -3318,7 +3447,7 @@
         <v>11</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>17</v>
@@ -3347,7 +3476,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>17</v>
@@ -3376,7 +3505,7 @@
         <v>11</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>17</v>
@@ -3405,7 +3534,7 @@
         <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>17</v>
@@ -3434,7 +3563,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>17</v>
@@ -3460,13 +3589,13 @@
         <v>49</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>19</v>
@@ -3492,10 +3621,10 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>19</v>
@@ -3518,13 +3647,13 @@
         <v>49</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>19</v>
@@ -3550,7 +3679,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>51</v>
@@ -3575,11 +3704,11 @@
       <c r="B97" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>51</v>
@@ -3604,11 +3733,11 @@
       <c r="B98" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>51</v>
@@ -3633,17 +3762,17 @@
       <c r="B99" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>7</v>
+      <c r="C99" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -3662,17 +3791,17 @@
       <c r="B100" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>7</v>
+      <c r="C100" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -3691,17 +3820,17 @@
       <c r="B101" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>11</v>
+      <c r="C101" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -3720,17 +3849,17 @@
       <c r="B102" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C102" s="5" t="s">
-        <v>11</v>
+      <c r="C102" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -3753,7 +3882,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>26</v>
@@ -3779,16 +3908,16 @@
         <v>49</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
@@ -3811,13 +3940,13 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -3837,13 +3966,13 @@
         <v>49</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>10</v>
@@ -3869,13 +3998,13 @@
         <v>11</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -3898,13 +4027,13 @@
         <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -3927,13 +4056,13 @@
         <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -3956,7 +4085,7 @@
         <v>11</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>57</v>
@@ -3985,13 +4114,13 @@
         <v>11</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
@@ -4014,13 +4143,13 @@
         <v>11</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
@@ -4043,13 +4172,13 @@
         <v>11</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -4060,34 +4189,34 @@
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
     </row>
-    <row r="114" spans="1:14" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="20">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="B114" s="13" t="s">
+      <c r="B114" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C114" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E114" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F114" s="13" t="s">
+      <c r="C114" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G114" s="13"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-      <c r="J114" s="13"/>
-      <c r="K114" s="13"/>
-      <c r="L114" s="13"/>
-      <c r="M114" s="13"/>
-      <c r="N114" s="13"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
     </row>
     <row r="115" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="20">
@@ -4098,16 +4227,16 @@
         <v>49</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
@@ -4118,34 +4247,34 @@
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
     </row>
-    <row r="116" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="20">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C116" s="5" t="s">
+      <c r="C116" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E116" s="2" t="s">
+      <c r="D116" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E116" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2"/>
-      <c r="N116" s="2"/>
+      <c r="F116" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13"/>
+      <c r="L116" s="13"/>
+      <c r="M116" s="13"/>
+      <c r="N116" s="13"/>
     </row>
     <row r="117" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="20">
@@ -4159,7 +4288,7 @@
         <v>7</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>9</v>
@@ -4188,7 +4317,7 @@
         <v>7</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>9</v>
@@ -4217,7 +4346,7 @@
         <v>7</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>9</v>
@@ -4239,29 +4368,29 @@
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D120" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E120" s="3" t="s">
+      <c r="D120" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E120" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F120" s="6" t="s">
+      <c r="F120" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="3"/>
-      <c r="L120" s="3"/>
-      <c r="M120" s="3"/>
-      <c r="N120" s="3"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2"/>
     </row>
     <row r="121" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="20">
@@ -4272,16 +4401,16 @@
         <v>49</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D121" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E121" s="15" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
@@ -4297,20 +4426,20 @@
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C122" s="2" t="s">
+      <c r="B122" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C122" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E122" s="2" t="s">
+      <c r="D122" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>10</v>
+      <c r="F122" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
@@ -4327,28 +4456,28 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E123" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="3"/>
-      <c r="K123" s="3"/>
-      <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+      <c r="N123" s="2"/>
     </row>
     <row r="124" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="20">
@@ -4356,28 +4485,28 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C124" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C124" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D124" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>17</v>
+      <c r="D124" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E124" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
-      <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2"/>
+      <c r="M124" s="2"/>
+      <c r="N124" s="2"/>
     </row>
     <row r="125" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="20">
@@ -4388,16 +4517,16 @@
         <v>70</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D125" s="10" t="s">
-        <v>84</v>
+        <v>7</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
@@ -4417,13 +4546,13 @@
         <v>70</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>19</v>
@@ -4449,7 +4578,7 @@
         <v>11</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>17</v>
@@ -4477,8 +4606,8 @@
       <c r="C128" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>22</v>
+      <c r="D128" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>17</v>
@@ -4507,7 +4636,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>17</v>
@@ -4536,7 +4665,7 @@
         <v>11</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>17</v>
@@ -4555,20 +4684,20 @@
     </row>
     <row r="131" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="20">
-        <f t="shared" ref="A131:A159" si="2">ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>19</v>
@@ -4584,7 +4713,7 @@
     </row>
     <row r="132" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -4594,10 +4723,10 @@
         <v>11</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>19</v>
@@ -4613,7 +4742,7 @@
     </row>
     <row r="133" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
@@ -4623,10 +4752,10 @@
         <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>19</v>
@@ -4642,20 +4771,20 @@
     </row>
     <row r="134" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A134:A163" si="2">ROW() - 1</f>
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>19</v>
@@ -4677,11 +4806,11 @@
       <c r="B135" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="C135" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>51</v>
@@ -4706,11 +4835,11 @@
       <c r="B136" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C136" s="5" t="s">
+      <c r="C136" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>51</v>
@@ -4736,16 +4865,16 @@
         <v>70</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
@@ -4764,17 +4893,17 @@
       <c r="B138" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>7</v>
+      <c r="C138" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
@@ -4797,10 +4926,10 @@
         <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>19</v>
@@ -4822,17 +4951,17 @@
       <c r="B140" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C140" s="5" t="s">
-        <v>11</v>
+      <c r="C140" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
@@ -4851,17 +4980,17 @@
       <c r="B141" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C141" s="5" t="s">
-        <v>11</v>
+      <c r="C141" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
@@ -4881,16 +5010,16 @@
         <v>70</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
@@ -4913,13 +5042,13 @@
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
@@ -4942,13 +5071,13 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
@@ -4968,16 +5097,16 @@
         <v>70</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
@@ -5000,22 +5129,22 @@
         <v>11</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
-      <c r="I146" s="2"/>
-      <c r="J146" s="2"/>
-      <c r="K146" s="2"/>
-      <c r="L146" s="2"/>
-      <c r="M146" s="2"/>
-      <c r="N146" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G146" s="3"/>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
     </row>
     <row r="147" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="20">
@@ -5029,7 +5158,7 @@
         <v>11</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>57</v>
@@ -5037,14 +5166,14 @@
       <c r="F147" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
-      <c r="L147" s="2"/>
-      <c r="M147" s="2"/>
-      <c r="N147" s="2"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="3"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
     </row>
     <row r="148" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="20">
@@ -5058,7 +5187,7 @@
         <v>11</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>57</v>
@@ -5066,14 +5195,14 @@
       <c r="F148" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-      <c r="L148" s="2"/>
-      <c r="M148" s="2"/>
-      <c r="N148" s="2"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
     </row>
     <row r="149" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="20">
@@ -5087,7 +5216,7 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>57</v>
@@ -5116,7 +5245,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>57</v>
@@ -5145,13 +5274,13 @@
         <v>11</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
@@ -5170,17 +5299,17 @@
       <c r="B152" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>7</v>
+      <c r="C152" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
@@ -5200,16 +5329,16 @@
         <v>70</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D153" s="10" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
@@ -5229,16 +5358,16 @@
         <v>70</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
@@ -5260,14 +5389,14 @@
       <c r="C155" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D155" s="10" t="s">
-        <v>67</v>
+      <c r="D155" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
@@ -5289,8 +5418,8 @@
       <c r="C156" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D156" s="3" t="s">
-        <v>68</v>
+      <c r="D156" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>9</v>
@@ -5319,7 +5448,7 @@
         <v>7</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>9</v>
@@ -5344,17 +5473,17 @@
       <c r="B158" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C158" s="5" t="s">
-        <v>11</v>
+      <c r="C158" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D158" s="10" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
@@ -5374,16 +5503,16 @@
         <v>70</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D159" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E159" s="15" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
@@ -5395,12 +5524,25 @@
       <c r="N159" s="2"/>
     </row>
     <row r="160" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A160" s="20"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="5"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
+      <c r="A160" s="20">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
@@ -5411,12 +5553,25 @@
       <c r="N160" s="2"/>
     </row>
     <row r="161" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A161" s="20"/>
-      <c r="B161" s="2"/>
-      <c r="C161" s="5"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
+      <c r="A161" s="20">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G161" s="2"/>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -5427,12 +5582,25 @@
       <c r="N161" s="2"/>
     </row>
     <row r="162" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A162" s="20"/>
-      <c r="B162" s="2"/>
-      <c r="C162" s="5"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
+      <c r="A162" s="20">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E162" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -5443,12 +5611,25 @@
       <c r="N162" s="2"/>
     </row>
     <row r="163" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A163" s="20"/>
-      <c r="B163" s="2"/>
-      <c r="C163" s="5"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
+      <c r="A163" s="20">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E163" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G163" s="2"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
@@ -5461,7 +5642,7 @@
     <row r="164" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="20"/>
       <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
+      <c r="C164" s="5"/>
       <c r="D164" s="3"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
@@ -5509,7 +5690,7 @@
     <row r="167" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="20"/>
       <c r="B167" s="2"/>
-      <c r="C167" s="5"/>
+      <c r="C167" s="2"/>
       <c r="D167" s="3"/>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
@@ -5541,8 +5722,8 @@
     <row r="169" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="20"/>
       <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-      <c r="D169" s="2"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="3"/>
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
@@ -5557,8 +5738,8 @@
     <row r="170" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-      <c r="D170" s="2"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="3"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
@@ -5573,8 +5754,8 @@
     <row r="171" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
-      <c r="D171" s="2"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="3"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
@@ -18274,6 +18455,54 @@
       <c r="M964" s="2"/>
       <c r="N964" s="2"/>
     </row>
+    <row r="965" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A965" s="20"/>
+      <c r="B965" s="2"/>
+      <c r="C965" s="2"/>
+      <c r="D965" s="2"/>
+      <c r="E965" s="2"/>
+      <c r="F965" s="2"/>
+      <c r="G965" s="2"/>
+      <c r="H965" s="2"/>
+      <c r="I965" s="2"/>
+      <c r="J965" s="2"/>
+      <c r="K965" s="2"/>
+      <c r="L965" s="2"/>
+      <c r="M965" s="2"/>
+      <c r="N965" s="2"/>
+    </row>
+    <row r="966" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A966" s="20"/>
+      <c r="B966" s="2"/>
+      <c r="C966" s="2"/>
+      <c r="D966" s="2"/>
+      <c r="E966" s="2"/>
+      <c r="F966" s="2"/>
+      <c r="G966" s="2"/>
+      <c r="H966" s="2"/>
+      <c r="I966" s="2"/>
+      <c r="J966" s="2"/>
+      <c r="K966" s="2"/>
+      <c r="L966" s="2"/>
+      <c r="M966" s="2"/>
+      <c r="N966" s="2"/>
+    </row>
+    <row r="967" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A967" s="20"/>
+      <c r="B967" s="2"/>
+      <c r="C967" s="2"/>
+      <c r="D967" s="2"/>
+      <c r="E967" s="2"/>
+      <c r="F967" s="2"/>
+      <c r="G967" s="2"/>
+      <c r="H967" s="2"/>
+      <c r="I967" s="2"/>
+      <c r="J967" s="2"/>
+      <c r="K967" s="2"/>
+      <c r="L967" s="2"/>
+      <c r="M967" s="2"/>
+      <c r="N967" s="2"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
@@ -18281,48 +18510,92 @@
       <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F82:F120 F122:F158 F160:F964 F1:F80">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Read">
+  <conditionalFormatting sqref="F83:F84 F125:F161 F164:F967 F1:F34 F36:F81 F86:F122">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH(("No"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Write">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Write">
       <formula>NOT(ISERROR(SEARCH(("Write"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F81">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F81))))</formula>
+  <conditionalFormatting sqref="F82">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F82))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F81))))</formula>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F82))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F81))))</formula>
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F82))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F121">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F121))))</formula>
+  <conditionalFormatting sqref="F123">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F123))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F121))))</formula>
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F123))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F121))))</formula>
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F123))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F159">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F159))))</formula>
+  <conditionalFormatting sqref="F162">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F162))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F159))))</formula>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F162))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F159))))</formula>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F162))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F35))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F35))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F85">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F85))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F85))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F85))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F124">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F124))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F124))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F124))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F163">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F163))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F163))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F163))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18338,13 +18611,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>ScreenIds!$B$2:$B$73</xm:f>
+            <xm:f>ScreenIds!$B$2:$B$76</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>ScreenIds!$B$3:$B$73</xm:f>
+            <xm:f>ScreenIds!$B$3:$B$76</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -18371,16 +18644,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
@@ -18782,6 +19055,21 @@
     <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="11" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OP-1841 and Rebasing with document repository
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LexCheck\WEB\role-permission-binish\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141A76D0-6776-4F52-96E0-55E0678A9C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C1C7E0-154D-465A-A121-5AFD6437F45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="permissions" sheetId="1" r:id="rId1"/>
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$967</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$973</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="90">
   <si>
     <t>User</t>
   </si>
@@ -302,6 +302,15 @@
   <si>
     <t>document-repository-comp</t>
   </si>
+  <si>
+    <t>customer-management-comp</t>
+  </si>
+  <si>
+    <t>document-management-comp</t>
+  </si>
+  <si>
+    <t>platform-insights-comp</t>
+  </si>
 </sst>
 </file>
 
@@ -452,79 +461,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -763,10 +700,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N967"/>
+  <dimension ref="A1:N973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="F163" sqref="A1:F163"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="139" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -837,7 +774,7 @@
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
-        <f t="shared" ref="A3:A67" si="0">ROW() - 1</f>
+        <f t="shared" ref="A3:A68" si="0">ROW() - 1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1764,81 +1701,81 @@
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
+      <c r="A35" s="17">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <f t="shared" si="0"/>
+      <c r="A36" s="18">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>42</v>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>19</v>
+      <c r="F37" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -1861,13 +1798,13 @@
         <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1890,7 +1827,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>9</v>
@@ -1916,16 +1853,16 @@
         <v>42</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -1948,7 +1885,7 @@
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>17</v>
@@ -1977,7 +1914,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>17</v>
@@ -2006,7 +1943,7 @@
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>17</v>
@@ -2035,13 +1972,13 @@
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2060,17 +1997,17 @@
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2093,7 +2030,7 @@
         <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>17</v>
@@ -2118,11 +2055,11 @@
       <c r="B47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>17</v>
@@ -2145,19 +2082,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -2177,13 +2114,13 @@
         <v>44</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>10</v>
@@ -2209,10 +2146,10 @@
         <v>11</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="13" t="s">
         <v>13</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>10</v>
@@ -2237,8 +2174,8 @@
       <c r="C51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>14</v>
+      <c r="D51" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>13</v>
@@ -2260,17 +2197,17 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>10</v>
@@ -2289,14 +2226,14 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>15</v>
+      <c r="D53" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>8</v>
@@ -2325,9 +2262,9 @@
         <v>11</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
@@ -2351,16 +2288,16 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -2380,13 +2317,13 @@
         <v>44</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>19</v>
@@ -2412,7 +2349,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>17</v>
@@ -2441,7 +2378,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>17</v>
@@ -2470,7 +2407,7 @@
         <v>11</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>17</v>
@@ -2499,7 +2436,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>17</v>
@@ -2528,7 +2465,7 @@
         <v>11</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>17</v>
@@ -2557,7 +2494,7 @@
         <v>11</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>17</v>
@@ -2583,16 +2520,16 @@
         <v>44</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -2615,7 +2552,7 @@
         <v>7</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>9</v>
@@ -2641,16 +2578,16 @@
         <v>44</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -2669,11 +2606,11 @@
       <c r="B66" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>26</v>
@@ -2702,7 +2639,7 @@
         <v>11</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>26</v>
@@ -2721,23 +2658,23 @@
     </row>
     <row r="68" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
-        <f t="shared" ref="A68:A133" si="1">ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>7</v>
+      <c r="C68" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -2750,20 +2687,20 @@
     </row>
     <row r="69" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A69:A139" si="1">ROW() - 1</f>
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>10</v>
@@ -2789,13 +2726,13 @@
         <v>11</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2818,13 +2755,13 @@
         <v>11</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2844,16 +2781,16 @@
         <v>44</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -2872,14 +2809,14 @@
       <c r="B73" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>11</v>
+      <c r="C73" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>19</v>
@@ -2905,7 +2842,7 @@
         <v>11</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>45</v>
@@ -2934,7 +2871,7 @@
         <v>11</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>45</v>
@@ -2960,13 +2897,13 @@
         <v>44</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>19</v>
@@ -2989,16 +2926,16 @@
         <v>44</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -3021,10 +2958,10 @@
         <v>11</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>10</v>
@@ -3050,13 +2987,13 @@
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3079,13 +3016,13 @@
         <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3108,10 +3045,10 @@
         <v>11</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>10</v>
@@ -3136,11 +3073,11 @@
       <c r="C82" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>33</v>
+      <c r="D82" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>10</v>
@@ -3165,11 +3102,11 @@
       <c r="C83" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>35</v>
+      <c r="D83" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>10</v>
@@ -3195,10 +3132,10 @@
         <v>11</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>10</v>
@@ -3213,20 +3150,21 @@
       <c r="N84" s="2"/>
     </row>
     <row r="85" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A85" s="18">
+      <c r="A85" s="17">
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>7</v>
+      <c r="C85" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>10</v>
@@ -3242,23 +3180,22 @@
     </row>
     <row r="86" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
-        <f t="shared" si="1"/>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C86" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -3270,24 +3207,23 @@
       <c r="N86" s="2"/>
     </row>
     <row r="87" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A87" s="17">
-        <f t="shared" si="1"/>
+      <c r="A87" s="18">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -3307,16 +3243,16 @@
         <v>49</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -3336,13 +3272,13 @@
         <v>49</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>19</v>
@@ -3368,7 +3304,7 @@
         <v>11</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>17</v>
@@ -3397,7 +3333,7 @@
         <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>17</v>
@@ -3426,7 +3362,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>17</v>
@@ -3455,7 +3391,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>17</v>
@@ -3484,7 +3420,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>17</v>
@@ -3510,13 +3446,13 @@
         <v>49</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>19</v>
@@ -3542,10 +3478,10 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>19</v>
@@ -3561,20 +3497,19 @@
     </row>
     <row r="97" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
-        <f t="shared" si="1"/>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>19</v>
@@ -3590,20 +3525,19 @@
     </row>
     <row r="98" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
-        <f t="shared" si="1"/>
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>19</v>
@@ -3619,20 +3553,19 @@
     </row>
     <row r="99" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
-        <f t="shared" si="1"/>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>11</v>
+      <c r="C99" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>19</v>
@@ -3654,14 +3587,14 @@
       <c r="B100" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>11</v>
+      <c r="C100" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>19</v>
@@ -3684,16 +3617,16 @@
         <v>49</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -3713,16 +3646,16 @@
         <v>49</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -3741,14 +3674,14 @@
       <c r="B103" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>19</v>
@@ -3774,10 +3707,10 @@
         <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>19</v>
@@ -3803,10 +3736,10 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>19</v>
@@ -3828,14 +3761,14 @@
       <c r="B106" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C106" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>10</v>
@@ -3857,14 +3790,14 @@
       <c r="B107" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>11</v>
+      <c r="C107" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>10</v>
@@ -3890,13 +3823,13 @@
         <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -3919,10 +3852,10 @@
         <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>19</v>
@@ -3948,10 +3881,10 @@
         <v>11</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>19</v>
@@ -3974,13 +3907,13 @@
         <v>49</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>10</v>
@@ -4006,13 +3939,13 @@
         <v>11</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
@@ -4035,13 +3968,13 @@
         <v>11</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -4064,13 +3997,13 @@
         <v>11</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
@@ -4093,13 +4026,13 @@
         <v>11</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
@@ -4118,14 +4051,14 @@
       <c r="B116" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>7</v>
+      <c r="C116" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>10</v>
@@ -4148,13 +4081,13 @@
         <v>49</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>19</v>
@@ -4177,13 +4110,13 @@
         <v>49</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>19</v>
@@ -4206,16 +4139,16 @@
         <v>49</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
@@ -4235,25 +4168,25 @@
         <v>49</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="3"/>
-      <c r="L120" s="3"/>
-      <c r="M120" s="3"/>
-      <c r="N120" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2"/>
     </row>
     <row r="121" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
@@ -4263,17 +4196,17 @@
       <c r="B121" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="C121" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
@@ -4289,29 +4222,29 @@
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D122" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E122" s="3" t="s">
+      <c r="D122" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="6" t="s">
+      <c r="F122" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+      <c r="N122" s="2"/>
     </row>
     <row r="123" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
@@ -4322,53 +4255,54 @@
         <v>49</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D123" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E123" s="13" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="3"/>
-      <c r="K123" s="3"/>
-      <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+      <c r="N123" s="2"/>
     </row>
     <row r="124" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="17">
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
-      <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2"/>
+      <c r="M124" s="2"/>
+      <c r="N124" s="2"/>
     </row>
     <row r="125" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="17">
@@ -4376,19 +4310,19 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C125" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C125" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
@@ -4405,13 +4339,13 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C126" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C126" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
@@ -4419,33 +4353,33 @@
       <c r="F126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G126" s="3"/>
-      <c r="H126" s="3"/>
-      <c r="I126" s="3"/>
-      <c r="J126" s="3"/>
-      <c r="K126" s="3"/>
-      <c r="L126" s="3"/>
-      <c r="M126" s="3"/>
-      <c r="N126" s="3"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+      <c r="L126" s="2"/>
+      <c r="M126" s="2"/>
+      <c r="N126" s="2"/>
     </row>
     <row r="127" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F127" s="2" t="s">
+      <c r="B127" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F127" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G127" s="3"/>
@@ -4463,19 +4397,19 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C128" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C128" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>17</v>
+        <v>77</v>
+      </c>
+      <c r="E128" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
@@ -4488,23 +4422,22 @@
     </row>
     <row r="129" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
-        <f t="shared" si="1"/>
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
@@ -4524,16 +4457,16 @@
         <v>70</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
@@ -4553,17 +4486,15 @@
         <v>70</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F131" s="2"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
@@ -4582,13 +4513,13 @@
         <v>70</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>19</v>
@@ -4614,7 +4545,7 @@
         <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>17</v>
@@ -4633,20 +4564,20 @@
     </row>
     <row r="134" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="17">
-        <f t="shared" ref="A134:A163" si="2">ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="D134" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>19</v>
@@ -4662,7 +4593,7 @@
     </row>
     <row r="135" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
@@ -4672,10 +4603,10 @@
         <v>11</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>19</v>
@@ -4691,7 +4622,7 @@
     </row>
     <row r="136" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
@@ -4701,10 +4632,10 @@
         <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>19</v>
@@ -4720,7 +4651,7 @@
     </row>
     <row r="137" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
@@ -4730,10 +4661,10 @@
         <v>11</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>19</v>
@@ -4749,20 +4680,20 @@
     </row>
     <row r="138" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>19</v>
@@ -4778,20 +4709,20 @@
     </row>
     <row r="139" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C139" s="5" t="s">
+      <c r="C139" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>19</v>
@@ -4807,7 +4738,7 @@
     </row>
     <row r="140" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A140:A169" si="2">ROW() - 1</f>
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -4817,13 +4748,13 @@
         <v>7</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
@@ -4843,16 +4774,16 @@
         <v>70</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
@@ -4871,14 +4802,14 @@
       <c r="B142" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C142" s="5" t="s">
+      <c r="C142" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>19</v>
@@ -4900,14 +4831,14 @@
       <c r="B143" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C143" s="5" t="s">
+      <c r="C143" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>19</v>
@@ -4933,10 +4864,10 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>19</v>
@@ -4959,16 +4890,16 @@
         <v>70</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
@@ -4987,14 +4918,14 @@
       <c r="B146" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C146" s="5" t="s">
-        <v>11</v>
+      <c r="C146" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>10</v>
@@ -5016,26 +4947,26 @@
       <c r="B147" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C147" s="5" t="s">
-        <v>11</v>
+      <c r="C147" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
-      <c r="L147" s="2"/>
-      <c r="M147" s="2"/>
-      <c r="N147" s="2"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="3"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
     </row>
     <row r="148" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="17">
@@ -5049,22 +4980,22 @@
         <v>11</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-      <c r="L148" s="2"/>
-      <c r="M148" s="2"/>
-      <c r="N148" s="2"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
     </row>
     <row r="149" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="17">
@@ -5078,22 +5009,22 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
-      <c r="J149" s="2"/>
-      <c r="K149" s="2"/>
-      <c r="L149" s="2"/>
-      <c r="M149" s="2"/>
-      <c r="N149" s="2"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
     </row>
     <row r="150" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="17">
@@ -5107,22 +5038,22 @@
         <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
-      <c r="J150" s="2"/>
-      <c r="K150" s="2"/>
-      <c r="L150" s="2"/>
-      <c r="M150" s="2"/>
-      <c r="N150" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="G150" s="3"/>
+      <c r="H150" s="3"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3"/>
     </row>
     <row r="151" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="17">
@@ -5133,25 +5064,25 @@
         <v>70</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
-      <c r="K151" s="2"/>
-      <c r="L151" s="2"/>
-      <c r="M151" s="2"/>
-      <c r="N151" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G151" s="3"/>
+      <c r="H151" s="3"/>
+      <c r="I151" s="3"/>
+      <c r="J151" s="3"/>
+      <c r="K151" s="3"/>
+      <c r="L151" s="3"/>
+      <c r="M151" s="3"/>
+      <c r="N151" s="3"/>
     </row>
     <row r="152" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="17">
@@ -5165,22 +5096,22 @@
         <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
-      <c r="I152" s="2"/>
-      <c r="J152" s="2"/>
-      <c r="K152" s="2"/>
-      <c r="L152" s="2"/>
-      <c r="M152" s="2"/>
-      <c r="N152" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G152" s="3"/>
+      <c r="H152" s="3"/>
+      <c r="I152" s="3"/>
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+      <c r="L152" s="3"/>
+      <c r="M152" s="3"/>
+      <c r="N152" s="3"/>
     </row>
     <row r="153" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="17">
@@ -5194,7 +5125,7 @@
         <v>11</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>57</v>
@@ -5223,13 +5154,13 @@
         <v>11</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
@@ -5248,17 +5179,17 @@
       <c r="B155" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>7</v>
+      <c r="C155" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
@@ -5278,16 +5209,16 @@
         <v>70</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D156" s="10" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
@@ -5307,13 +5238,13 @@
         <v>70</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>19</v>
@@ -5335,14 +5266,14 @@
       <c r="B158" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C158" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D158" s="10" t="s">
-        <v>67</v>
+      <c r="C158" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>19</v>
@@ -5365,16 +5296,16 @@
         <v>70</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
@@ -5394,16 +5325,16 @@
         <v>70</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
@@ -5422,14 +5353,14 @@
       <c r="B161" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C161" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D161" s="10" t="s">
-        <v>83</v>
+      <c r="C161" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>10</v>
@@ -5452,16 +5383,16 @@
         <v>70</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D162" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E162" s="13" t="s">
-        <v>61</v>
+        <v>85</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
@@ -5480,18 +5411,19 @@
       <c r="B163" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C163" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G163" s="2"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
       <c r="J163" s="2"/>
@@ -5501,12 +5433,25 @@
       <c r="N163" s="2"/>
     </row>
     <row r="164" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A164" s="17"/>
-      <c r="B164" s="2"/>
-      <c r="C164" s="5"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="2"/>
-      <c r="F164" s="2"/>
+      <c r="A164" s="17">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
       <c r="I164" s="2"/>
@@ -5517,12 +5462,25 @@
       <c r="N164" s="2"/>
     </row>
     <row r="165" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A165" s="17"/>
-      <c r="B165" s="2"/>
-      <c r="C165" s="5"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="2"/>
-      <c r="F165" s="2"/>
+      <c r="A165" s="17">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
@@ -5533,12 +5491,25 @@
       <c r="N165" s="2"/>
     </row>
     <row r="166" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A166" s="17"/>
-      <c r="B166" s="2"/>
-      <c r="C166" s="5"/>
-      <c r="D166" s="3"/>
-      <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
+      <c r="A166" s="17">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
@@ -5549,12 +5520,25 @@
       <c r="N166" s="2"/>
     </row>
     <row r="167" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A167" s="17"/>
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="3"/>
-      <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
+      <c r="A167" s="17">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D167" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G167" s="2"/>
       <c r="H167" s="2"/>
       <c r="I167" s="2"/>
@@ -5565,12 +5549,25 @@
       <c r="N167" s="2"/>
     </row>
     <row r="168" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A168" s="17"/>
-      <c r="B168" s="2"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="3"/>
-      <c r="E168" s="2"/>
-      <c r="F168" s="2"/>
+      <c r="A168" s="17">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E168" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
       <c r="I168" s="2"/>
@@ -5581,13 +5578,25 @@
       <c r="N168" s="2"/>
     </row>
     <row r="169" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A169" s="17"/>
-      <c r="B169" s="2"/>
-      <c r="C169" s="5"/>
-      <c r="D169" s="3"/>
-      <c r="E169" s="2"/>
-      <c r="F169" s="2"/>
-      <c r="G169" s="2"/>
+      <c r="A169" s="17">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
       <c r="J169" s="2"/>
@@ -5631,8 +5640,8 @@
     <row r="172" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="17"/>
       <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
-      <c r="D172" s="2"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="3"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
@@ -5648,7 +5657,7 @@
       <c r="A173" s="17"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
-      <c r="D173" s="2"/>
+      <c r="D173" s="3"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
@@ -5663,8 +5672,8 @@
     <row r="174" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="17"/>
       <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="2"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="3"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
@@ -5679,8 +5688,8 @@
     <row r="175" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="17"/>
       <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-      <c r="D175" s="2"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="3"/>
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
@@ -5695,8 +5704,8 @@
     <row r="176" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="17"/>
       <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
-      <c r="D176" s="2"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="3"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -5711,8 +5720,8 @@
     <row r="177" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="17"/>
       <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
-      <c r="D177" s="2"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="3"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
@@ -18332,71 +18341,134 @@
       <c r="M965" s="2"/>
       <c r="N965" s="2"/>
     </row>
-    <row r="966" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="966" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A966" s="17"/>
       <c r="B966" s="2"/>
       <c r="C966" s="2"/>
       <c r="D966" s="2"/>
       <c r="E966" s="2"/>
       <c r="F966" s="2"/>
-    </row>
-    <row r="967" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G966" s="2"/>
+      <c r="H966" s="2"/>
+      <c r="I966" s="2"/>
+      <c r="J966" s="2"/>
+      <c r="K966" s="2"/>
+      <c r="L966" s="2"/>
+      <c r="M966" s="2"/>
+      <c r="N966" s="2"/>
+    </row>
+    <row r="967" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A967" s="17"/>
       <c r="B967" s="2"/>
       <c r="C967" s="2"/>
       <c r="D967" s="2"/>
       <c r="E967" s="2"/>
       <c r="F967" s="2"/>
+      <c r="G967" s="2"/>
+      <c r="H967" s="2"/>
+      <c r="I967" s="2"/>
+      <c r="J967" s="2"/>
+      <c r="K967" s="2"/>
+      <c r="L967" s="2"/>
+      <c r="M967" s="2"/>
+      <c r="N967" s="2"/>
+    </row>
+    <row r="968" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A968" s="17"/>
+      <c r="B968" s="2"/>
+      <c r="C968" s="2"/>
+      <c r="D968" s="2"/>
+      <c r="E968" s="2"/>
+      <c r="F968" s="2"/>
+      <c r="G968" s="2"/>
+      <c r="H968" s="2"/>
+      <c r="I968" s="2"/>
+      <c r="J968" s="2"/>
+      <c r="K968" s="2"/>
+      <c r="L968" s="2"/>
+      <c r="M968" s="2"/>
+      <c r="N968" s="2"/>
+    </row>
+    <row r="969" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A969" s="17"/>
+      <c r="B969" s="2"/>
+      <c r="C969" s="2"/>
+      <c r="D969" s="2"/>
+      <c r="E969" s="2"/>
+      <c r="F969" s="2"/>
+      <c r="G969" s="2"/>
+      <c r="H969" s="2"/>
+      <c r="I969" s="2"/>
+      <c r="J969" s="2"/>
+      <c r="K969" s="2"/>
+      <c r="L969" s="2"/>
+      <c r="M969" s="2"/>
+      <c r="N969" s="2"/>
+    </row>
+    <row r="970" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A970" s="17"/>
+      <c r="B970" s="2"/>
+      <c r="C970" s="2"/>
+      <c r="D970" s="2"/>
+      <c r="E970" s="2"/>
+      <c r="F970" s="2"/>
+      <c r="G970" s="2"/>
+      <c r="H970" s="2"/>
+      <c r="I970" s="2"/>
+      <c r="J970" s="2"/>
+      <c r="K970" s="2"/>
+      <c r="L970" s="2"/>
+      <c r="M970" s="2"/>
+      <c r="N970" s="2"/>
+    </row>
+    <row r="971" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A971" s="17"/>
+      <c r="B971" s="2"/>
+      <c r="C971" s="2"/>
+      <c r="D971" s="2"/>
+      <c r="E971" s="2"/>
+      <c r="F971" s="2"/>
+      <c r="G971" s="2"/>
+      <c r="H971" s="2"/>
+      <c r="I971" s="2"/>
+      <c r="J971" s="2"/>
+      <c r="K971" s="2"/>
+      <c r="L971" s="2"/>
+      <c r="M971" s="2"/>
+      <c r="N971" s="2"/>
+    </row>
+    <row r="972" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A972" s="17"/>
+      <c r="B972" s="2"/>
+      <c r="C972" s="2"/>
+      <c r="D972" s="2"/>
+      <c r="E972" s="2"/>
+      <c r="F972" s="2"/>
+    </row>
+    <row r="973" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A973" s="17"/>
+      <c r="B973" s="2"/>
+      <c r="C973" s="2"/>
+      <c r="D973" s="2"/>
+      <c r="E973" s="2"/>
+      <c r="F973" s="2"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A950" xr:uid="{9E81345D-B4B2-485B-B238-1829345ECEE2}"/>
+      <autoFilter ref="A1:A950" xr:uid="{5214EAC6-C1CB-44B8-9242-9CCC865BA4A4}"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F1:F34 F36:F84 F86:F162 F164:F967">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Read">
+  <conditionalFormatting sqref="F1:F973">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH(("No"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Write">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Write">
       <formula>NOT(ISERROR(SEARCH(("Write"),(F1))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F35))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F35))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F85">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F85))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F85))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F85))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F163">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F163))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F163))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F163))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18408,31 +18480,31 @@
           <x14:formula1>
             <xm:f>ScreenIds!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B34 B36:B162 B164:B1048576</xm:sqref>
+          <xm:sqref>B37:B168 B170:B1048576 B1:B35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
-            <xm:f>ScreenIds!$B$2:$B$73</xm:f>
+            <xm:f>ScreenIds!$B$2:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E34 E36:E84 E86:E162 E164:E1048576</xm:sqref>
+          <xm:sqref>E1:E35 E37:E86 E170:E1048576 E88:E168</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>ScreenIds!$B$3:$B$73</xm:f>
+            <xm:f>ScreenIds!$B$3:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D34 D36:D84 D86:D123 D125:D162 D164:D1048576</xm:sqref>
+          <xm:sqref>D1:D35 D37:D86 D170:D1048576 D130:D168 D88:D128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F34 F36:F84 F86:F162 F164:F1048576</xm:sqref>
+          <xm:sqref>F1:F35 F37:F86 F170:F1048576 F88:F168</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C34 C36:C84 C86:C162 C164:C1048576</xm:sqref>
+          <xm:sqref>C1:C35 C37:C86 C170:C1048576 C88:C168</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18445,10 +18517,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18863,6 +18935,21 @@
         <v>86</v>
       </c>
     </row>
+    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B73">
     <sortCondition ref="B3"/>

</xml_diff>

<commit_message>
Adding role permissions for payment settings tab
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayesha.afzal\source\repos\role-permissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583C7B18-18DE-49C6-AD1F-7BBFA9D070B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA55836B-91DE-4FF1-B018-7FE5ABABAD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$973</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$974</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="91">
   <si>
     <t>User</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>platform-insights-comp</t>
+  </si>
+  <si>
+    <t>settings-comp</t>
   </si>
 </sst>
 </file>
@@ -700,10 +703,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N973"/>
+  <dimension ref="A1:N974"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="139" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="139" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2630,7 +2633,7 @@
     </row>
     <row r="67" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
-        <f t="shared" ref="A67:A101" si="1">ROW() - 1</f>
+        <f t="shared" ref="A67:A130" si="1">ROW() - 1</f>
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -3239,17 +3242,16 @@
     </row>
     <row r="88" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
-        <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C88" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>9</v>
@@ -3268,7 +3270,7 @@
     </row>
     <row r="89" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
-        <f t="shared" si="1"/>
+        <f>ROW() - 1</f>
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -3278,13 +3280,13 @@
         <v>7</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -3304,13 +3306,13 @@
         <v>49</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>19</v>
@@ -3336,7 +3338,7 @@
         <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>17</v>
@@ -3365,7 +3367,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>17</v>
@@ -3394,7 +3396,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>17</v>
@@ -3423,7 +3425,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>17</v>
@@ -3452,7 +3454,7 @@
         <v>11</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>17</v>
@@ -3481,7 +3483,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>17</v>
@@ -3507,13 +3509,13 @@
         <v>49</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>19</v>
@@ -3539,7 +3541,7 @@
         <v>7</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>9</v>
@@ -3568,7 +3570,7 @@
         <v>7</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>9</v>
@@ -3597,7 +3599,7 @@
         <v>7</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>9</v>
@@ -3623,13 +3625,13 @@
         <v>49</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>19</v>
@@ -3645,7 +3647,7 @@
     </row>
     <row r="102" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -3655,7 +3657,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>51</v>
@@ -3674,7 +3676,7 @@
     </row>
     <row r="103" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
-        <f t="shared" ref="A103:A166" si="2">ROW() - 1</f>
+        <f>ROW() - 1</f>
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
@@ -3684,7 +3686,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>51</v>
@@ -3703,17 +3705,17 @@
     </row>
     <row r="104" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A104:A167" si="2">ROW() - 1</f>
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C104" s="5" t="s">
+      <c r="C104" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>51</v>
@@ -3742,7 +3744,7 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>51</v>
@@ -3767,17 +3769,17 @@
       <c r="B106" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>7</v>
+      <c r="C106" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -3800,7 +3802,7 @@
         <v>7</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>9</v>
@@ -3825,17 +3827,17 @@
       <c r="B108" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>11</v>
+      <c r="C108" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -3858,7 +3860,7 @@
         <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>26</v>
@@ -3887,7 +3889,7 @@
         <v>11</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>26</v>
@@ -3913,16 +3915,16 @@
         <v>49</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
@@ -3942,13 +3944,13 @@
         <v>49</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>10</v>
@@ -3974,7 +3976,7 @@
         <v>11</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>57</v>
@@ -4003,13 +4005,13 @@
         <v>11</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
@@ -4032,7 +4034,7 @@
         <v>11</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>57</v>
@@ -4061,13 +4063,13 @@
         <v>11</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
@@ -4090,13 +4092,13 @@
         <v>11</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
@@ -4119,7 +4121,7 @@
         <v>11</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>57</v>
@@ -4148,13 +4150,13 @@
         <v>11</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
@@ -4177,7 +4179,7 @@
         <v>11</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>57</v>
@@ -4202,14 +4204,14 @@
       <c r="B121" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>7</v>
+      <c r="C121" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>10</v>
@@ -4231,17 +4233,17 @@
       <c r="B122" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C122" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
@@ -4261,10 +4263,10 @@
         <v>49</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>9</v>
@@ -4293,7 +4295,7 @@
         <v>11</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>9</v>
@@ -4322,7 +4324,7 @@
         <v>11</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>9</v>
@@ -4330,14 +4332,14 @@
       <c r="F125" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G125" s="3"/>
-      <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
-      <c r="J125" s="3"/>
-      <c r="K125" s="3"/>
-      <c r="L125" s="3"/>
-      <c r="M125" s="3"/>
-      <c r="N125" s="3"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2"/>
+      <c r="M125" s="2"/>
+      <c r="N125" s="2"/>
     </row>
     <row r="126" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="17">
@@ -4348,10 +4350,10 @@
         <v>49</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
@@ -4359,63 +4361,63 @@
       <c r="F126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-      <c r="J126" s="2"/>
-      <c r="K126" s="2"/>
-      <c r="L126" s="2"/>
-      <c r="M126" s="2"/>
-      <c r="N126" s="2"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="3"/>
+      <c r="N126" s="3"/>
     </row>
     <row r="127" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <f t="shared" si="2"/>
         <v>126</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D127" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E127" s="3" t="s">
+      <c r="D127" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F127" s="6" t="s">
+      <c r="F127" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G127" s="3"/>
-      <c r="H127" s="3"/>
-      <c r="I127" s="3"/>
-      <c r="J127" s="3"/>
-      <c r="K127" s="3"/>
-      <c r="L127" s="3"/>
-      <c r="M127" s="3"/>
-      <c r="N127" s="3"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+      <c r="L127" s="2"/>
+      <c r="M127" s="2"/>
+      <c r="N127" s="2"/>
     </row>
     <row r="128" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <f t="shared" si="2"/>
         <v>127</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C128" s="5" t="s">
-        <v>11</v>
+      <c r="C128" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E128" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>10</v>
+        <v>67</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
@@ -4434,14 +4436,14 @@
       <c r="B129" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>9</v>
+      <c r="D129" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E129" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>10</v>
@@ -4461,13 +4463,13 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>9</v>
@@ -4496,12 +4498,14 @@
         <v>7</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F131" s="2"/>
+      <c r="F131" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
@@ -4523,14 +4527,12 @@
         <v>7</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F132" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="F132" s="2"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
@@ -4549,13 +4551,13 @@
         <v>70</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>19</v>
@@ -4580,8 +4582,8 @@
       <c r="C134" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D134" s="10" t="s">
-        <v>84</v>
+      <c r="D134" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>17</v>
@@ -4609,8 +4611,8 @@
       <c r="C135" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>20</v>
+      <c r="D135" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>17</v>
@@ -4639,7 +4641,7 @@
         <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>17</v>
@@ -4668,7 +4670,7 @@
         <v>11</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>17</v>
@@ -4697,7 +4699,7 @@
         <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>17</v>
@@ -4726,7 +4728,7 @@
         <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>17</v>
@@ -4752,13 +4754,13 @@
         <v>70</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>19</v>
@@ -4781,13 +4783,13 @@
         <v>70</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>19</v>
@@ -4813,7 +4815,7 @@
         <v>11</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>51</v>
@@ -4842,7 +4844,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>51</v>
@@ -4867,11 +4869,11 @@
       <c r="B144" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C144" s="5" t="s">
+      <c r="C144" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>51</v>
@@ -4900,7 +4902,7 @@
         <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>51</v>
@@ -4925,17 +4927,17 @@
       <c r="B146" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>7</v>
+      <c r="C146" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
@@ -4958,7 +4960,7 @@
         <v>7</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>9</v>
@@ -4983,17 +4985,17 @@
       <c r="B148" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C148" s="5" t="s">
-        <v>11</v>
+      <c r="C148" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
@@ -5016,7 +5018,7 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>26</v>
@@ -5045,7 +5047,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>26</v>
@@ -5071,16 +5073,16 @@
         <v>70</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
@@ -5100,13 +5102,13 @@
         <v>70</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>10</v>
@@ -5132,7 +5134,7 @@
         <v>11</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>57</v>
@@ -5140,14 +5142,14 @@
       <c r="F153" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G153" s="2"/>
-      <c r="H153" s="2"/>
-      <c r="I153" s="2"/>
-      <c r="J153" s="2"/>
-      <c r="K153" s="2"/>
-      <c r="L153" s="2"/>
-      <c r="M153" s="2"/>
-      <c r="N153" s="2"/>
+      <c r="G153" s="3"/>
+      <c r="H153" s="3"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="3"/>
+      <c r="K153" s="3"/>
+      <c r="L153" s="3"/>
+      <c r="M153" s="3"/>
+      <c r="N153" s="3"/>
     </row>
     <row r="154" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="17">
@@ -5161,13 +5163,13 @@
         <v>11</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
@@ -5190,7 +5192,7 @@
         <v>11</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>57</v>
@@ -5219,13 +5221,13 @@
         <v>11</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
@@ -5248,13 +5250,13 @@
         <v>11</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
@@ -5277,7 +5279,7 @@
         <v>11</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>57</v>
@@ -5306,13 +5308,13 @@
         <v>11</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
@@ -5335,7 +5337,7 @@
         <v>11</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>57</v>
@@ -5360,14 +5362,14 @@
       <c r="B161" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>7</v>
+      <c r="C161" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>10</v>
@@ -5389,17 +5391,17 @@
       <c r="B162" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C162" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D162" s="10" t="s">
-        <v>85</v>
+      <c r="D162" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
@@ -5421,8 +5423,8 @@
       <c r="C163" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D163" s="3" t="s">
-        <v>71</v>
+      <c r="D163" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>9</v>
@@ -5448,10 +5450,10 @@
         <v>70</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D164" s="10" t="s">
-        <v>67</v>
+        <v>7</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>9</v>
@@ -5479,8 +5481,8 @@
       <c r="C165" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D165" s="3" t="s">
-        <v>68</v>
+      <c r="D165" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>9</v>
@@ -5509,7 +5511,7 @@
         <v>11</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>9</v>
@@ -5528,7 +5530,7 @@
     </row>
     <row r="167" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="17">
-        <f t="shared" ref="A167:A169" si="3">ROW() - 1</f>
+        <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
@@ -5537,14 +5539,14 @@
       <c r="C167" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D167" s="10" t="s">
-        <v>83</v>
+      <c r="D167" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G167" s="2"/>
       <c r="H167" s="2"/>
@@ -5557,7 +5559,7 @@
     </row>
     <row r="168" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A168:A170" si="3">ROW() - 1</f>
         <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
@@ -5567,10 +5569,10 @@
         <v>11</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E168" s="13" t="s">
-        <v>61</v>
+        <v>83</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>10</v>
@@ -5592,18 +5594,19 @@
       <c r="B169" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C169" s="3" t="s">
+      <c r="C169" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>9</v>
+      <c r="D169" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E169" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G169" s="2"/>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
       <c r="J169" s="2"/>
@@ -5613,13 +5616,25 @@
       <c r="N169" s="2"/>
     </row>
     <row r="170" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A170" s="17"/>
-      <c r="B170" s="2"/>
-      <c r="C170" s="5"/>
-      <c r="D170" s="3"/>
-      <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
-      <c r="G170" s="2"/>
+      <c r="A170" s="17">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
       <c r="J170" s="2"/>
@@ -5663,7 +5678,7 @@
     <row r="173" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="17"/>
       <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
+      <c r="C173" s="5"/>
       <c r="D173" s="3"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
@@ -5679,7 +5694,7 @@
     <row r="174" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="17"/>
       <c r="B174" s="2"/>
-      <c r="C174" s="5"/>
+      <c r="C174" s="2"/>
       <c r="D174" s="3"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
@@ -5743,8 +5758,8 @@
     <row r="178" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="17"/>
       <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
-      <c r="D178" s="2"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="3"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
@@ -18444,13 +18459,21 @@
       <c r="M971" s="2"/>
       <c r="N971" s="2"/>
     </row>
-    <row r="972" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="972" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A972" s="17"/>
       <c r="B972" s="2"/>
       <c r="C972" s="2"/>
       <c r="D972" s="2"/>
       <c r="E972" s="2"/>
       <c r="F972" s="2"/>
+      <c r="G972" s="2"/>
+      <c r="H972" s="2"/>
+      <c r="I972" s="2"/>
+      <c r="J972" s="2"/>
+      <c r="K972" s="2"/>
+      <c r="L972" s="2"/>
+      <c r="M972" s="2"/>
+      <c r="N972" s="2"/>
     </row>
     <row r="973" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A973" s="17"/>
@@ -18460,14 +18483,22 @@
       <c r="E973" s="2"/>
       <c r="F973" s="2"/>
     </row>
+    <row r="974" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A974" s="17"/>
+      <c r="B974" s="2"/>
+      <c r="C974" s="2"/>
+      <c r="D974" s="2"/>
+      <c r="E974" s="2"/>
+      <c r="F974" s="2"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A950" xr:uid="{AF24785D-747E-4A25-A011-0A5594846DF6}"/>
+      <autoFilter ref="A1:A950" xr:uid="{64A1C6BC-B890-4377-902D-BA3A539978EB}"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F1:F973">
+  <conditionalFormatting sqref="F1:F974">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
@@ -18487,31 +18518,31 @@
           <x14:formula1>
             <xm:f>ScreenIds!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B37:B168 B170:B1048576 B1:B35</xm:sqref>
+          <xm:sqref>B1:B35 B171:B1048576 B37:B169</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$B$2:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E35 E37:E86 E170:E1048576 E88:E168</xm:sqref>
+          <xm:sqref>E1:E35 E37:E86 E171:E1048576 E89:E169</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$B$3:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D35 D37:D86 D170:D1048576 D130:D168 D88:D128</xm:sqref>
+          <xm:sqref>D1:D35 D37:D86 D171:D1048576 D131:D169 D89:D129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F35 F37:F86 F170:F1048576 F88:F168</xm:sqref>
+          <xm:sqref>F1:F35 F37:F86 F171:F1048576 F89:F169</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C35 C37:C86 C170:C1048576 C88:C168</xm:sqref>
+          <xm:sqref>C1:C35 C37:C86 C171:C1048576 C88:C169</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18524,10 +18555,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18957,6 +18988,11 @@
         <v>89</v>
       </c>
     </row>
+    <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B73">
     <sortCondition ref="B3"/>

</xml_diff>

<commit_message>
Made sure all the permissions of Admin and Platfrom Admin are same.
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\permissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45807B65-24FC-4C80-9F9E-7422D6A1249D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
-    <sheet name="permissions" sheetId="1" r:id="rId1"/>
+    <sheet name="roles" sheetId="1" r:id="rId1"/>
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">permissions!$B$1:$B$979</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">roles!$B$1:$B$983</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{49968090-594F-4035-ABCC-088176AC5527}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="94">
   <si>
     <t>User</t>
   </si>
@@ -327,7 +326,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -485,7 +484,151 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -720,14 +863,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N979"/>
+  <dimension ref="A1:N983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="139" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3783,7 +3926,7 @@
     </row>
     <row r="106" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
-        <f t="shared" ref="A106:A172" si="3">ROW() - 1</f>
+        <f t="shared" ref="A106:A179" si="3">ROW() - 1</f>
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
@@ -4395,29 +4538,29 @@
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C127" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E127" s="2" t="s">
+      <c r="C127" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E127" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F127" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
-      <c r="J127" s="2"/>
-      <c r="K127" s="2"/>
-      <c r="L127" s="2"/>
-      <c r="M127" s="2"/>
-      <c r="N127" s="2"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="3"/>
+      <c r="K127" s="3"/>
+      <c r="L127" s="3"/>
+      <c r="M127" s="3"/>
+      <c r="N127" s="3"/>
     </row>
     <row r="128" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
@@ -4431,7 +4574,7 @@
         <v>11</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>9</v>
@@ -4439,14 +4582,14 @@
       <c r="F128" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G128" s="3"/>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="3"/>
-      <c r="K128" s="3"/>
-      <c r="L128" s="3"/>
-      <c r="M128" s="3"/>
-      <c r="N128" s="3"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+      <c r="L128" s="2"/>
+      <c r="M128" s="2"/>
+      <c r="N128" s="2"/>
     </row>
     <row r="129" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
@@ -4457,10 +4600,10 @@
         <v>49</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>9</v>
@@ -4468,43 +4611,43 @@
       <c r="F129" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
-      <c r="I129" s="2"/>
-      <c r="J129" s="2"/>
-      <c r="K129" s="2"/>
-      <c r="L129" s="2"/>
-      <c r="M129" s="2"/>
-      <c r="N129" s="2"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="3"/>
+      <c r="K129" s="3"/>
+      <c r="L129" s="3"/>
+      <c r="M129" s="3"/>
+      <c r="N129" s="3"/>
     </row>
     <row r="130" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="17">
         <f t="shared" si="3"/>
         <v>129</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B130" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C130" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D130" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E130" s="3" t="s">
+      <c r="D130" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E130" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F130" s="6" t="s">
+      <c r="F130" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G130" s="3"/>
-      <c r="H130" s="3"/>
-      <c r="I130" s="3"/>
-      <c r="J130" s="3"/>
-      <c r="K130" s="3"/>
-      <c r="L130" s="3"/>
-      <c r="M130" s="3"/>
-      <c r="N130" s="3"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2"/>
+      <c r="K130" s="2"/>
+      <c r="L130" s="2"/>
+      <c r="M130" s="2"/>
+      <c r="N130" s="2"/>
     </row>
     <row r="131" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="17">
@@ -4536,62 +4679,62 @@
       <c r="N131" s="3"/>
     </row>
     <row r="132" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A132" s="17">
+      <c r="A132" s="19">
         <f t="shared" si="3"/>
         <v>131</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D132" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F132" s="2" t="s">
+      <c r="D132" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E132" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F132" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G132" s="3"/>
-      <c r="H132" s="3"/>
-      <c r="I132" s="3"/>
-      <c r="J132" s="3"/>
-      <c r="K132" s="3"/>
-      <c r="L132" s="3"/>
-      <c r="M132" s="3"/>
-      <c r="N132" s="3"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="13"/>
+      <c r="J132" s="13"/>
+      <c r="K132" s="13"/>
+      <c r="L132" s="13"/>
+      <c r="M132" s="13"/>
+      <c r="N132" s="13"/>
     </row>
     <row r="133" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A133" s="19">
+      <c r="A133" s="17">
         <f t="shared" si="3"/>
         <v>132</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="B133" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C133" s="20" t="s">
+      <c r="C133" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D133" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E133" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F133" s="13" t="s">
+      <c r="D133" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F133" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G133" s="13"/>
-      <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
-      <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
-      <c r="L133" s="13"/>
-      <c r="M133" s="13"/>
-      <c r="N133" s="13"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="3"/>
+      <c r="K133" s="3"/>
+      <c r="L133" s="3"/>
+      <c r="M133" s="3"/>
+      <c r="N133" s="3"/>
     </row>
     <row r="134" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="17">
@@ -4599,28 +4742,28 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C134" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C134" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G134" s="3"/>
-      <c r="H134" s="3"/>
-      <c r="I134" s="3"/>
-      <c r="J134" s="3"/>
-      <c r="K134" s="3"/>
-      <c r="L134" s="3"/>
-      <c r="M134" s="3"/>
-      <c r="N134" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="2"/>
+      <c r="K134" s="2"/>
+      <c r="L134" s="2"/>
+      <c r="M134" s="2"/>
+      <c r="N134" s="2"/>
     </row>
     <row r="135" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="17">
@@ -4628,19 +4771,19 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>87</v>
+        <v>49</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
@@ -4663,7 +4806,7 @@
         <v>7</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>9</v>
@@ -4692,7 +4835,7 @@
         <v>7</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>9</v>
@@ -4700,14 +4843,14 @@
       <c r="F137" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-      <c r="K137" s="2"/>
-      <c r="L137" s="2"/>
-      <c r="M137" s="2"/>
-      <c r="N137" s="2"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
+      <c r="M137" s="3"/>
+      <c r="N137" s="3"/>
     </row>
     <row r="138" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
@@ -4718,13 +4861,13 @@
         <v>70</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E138" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>19</v>
@@ -4749,8 +4892,8 @@
       <c r="C139" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>18</v>
+      <c r="D139" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>17</v>
@@ -4778,8 +4921,8 @@
       <c r="C140" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D140" s="10" t="s">
-        <v>84</v>
+      <c r="D140" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>17</v>
@@ -4808,7 +4951,7 @@
         <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>17</v>
@@ -4837,7 +4980,7 @@
         <v>11</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>17</v>
@@ -4866,7 +5009,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>17</v>
@@ -4895,7 +5038,7 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>17</v>
@@ -4921,25 +5064,25 @@
         <v>70</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G145" s="3"/>
-      <c r="H145" s="3"/>
-      <c r="I145" s="3"/>
-      <c r="J145" s="3"/>
-      <c r="K145" s="3"/>
-      <c r="L145" s="3"/>
-      <c r="M145" s="3"/>
-      <c r="N145" s="3"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+      <c r="L145" s="2"/>
+      <c r="M145" s="2"/>
+      <c r="N145" s="2"/>
     </row>
     <row r="146" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
@@ -4953,13 +5096,13 @@
         <v>7</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
@@ -4979,25 +5122,25 @@
         <v>70</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G147" s="3"/>
-      <c r="H147" s="3"/>
-      <c r="I147" s="3"/>
-      <c r="J147" s="3"/>
-      <c r="K147" s="3"/>
-      <c r="L147" s="3"/>
-      <c r="M147" s="3"/>
-      <c r="N147" s="3"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+      <c r="L147" s="2"/>
+      <c r="M147" s="2"/>
+      <c r="N147" s="2"/>
     </row>
     <row r="148" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="17">
@@ -5008,13 +5151,13 @@
         <v>70</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>19</v>
@@ -5040,7 +5183,7 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>51</v>
@@ -5065,11 +5208,11 @@
       <c r="B150" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C150" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>51</v>
@@ -5094,11 +5237,11 @@
       <c r="B151" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C151" s="5" t="s">
+      <c r="C151" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>51</v>
@@ -5123,17 +5266,17 @@
       <c r="B152" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>7</v>
+      <c r="C152" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
@@ -5152,17 +5295,17 @@
       <c r="B153" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>7</v>
+      <c r="C153" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
@@ -5181,17 +5324,17 @@
       <c r="B154" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C154" s="5" t="s">
-        <v>11</v>
+      <c r="C154" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
@@ -5210,17 +5353,17 @@
       <c r="B155" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C155" s="5" t="s">
-        <v>11</v>
+      <c r="C155" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
@@ -5243,7 +5386,7 @@
         <v>11</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>26</v>
@@ -5269,16 +5412,16 @@
         <v>70</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
@@ -5301,13 +5444,13 @@
         <v>11</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
@@ -5327,25 +5470,25 @@
         <v>70</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
-      <c r="I159" s="2"/>
-      <c r="J159" s="2"/>
-      <c r="K159" s="2"/>
-      <c r="L159" s="2"/>
-      <c r="M159" s="2"/>
-      <c r="N159" s="2"/>
+      <c r="G159" s="3"/>
+      <c r="H159" s="3"/>
+      <c r="I159" s="3"/>
+      <c r="J159" s="3"/>
+      <c r="K159" s="3"/>
+      <c r="L159" s="3"/>
+      <c r="M159" s="3"/>
+      <c r="N159" s="3"/>
     </row>
     <row r="160" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="17">
@@ -5359,22 +5502,22 @@
         <v>11</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-      <c r="I160" s="2"/>
-      <c r="J160" s="2"/>
-      <c r="K160" s="2"/>
-      <c r="L160" s="2"/>
-      <c r="M160" s="2"/>
-      <c r="N160" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G160" s="3"/>
+      <c r="H160" s="3"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="3"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
     </row>
     <row r="161" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="17">
@@ -5388,13 +5531,13 @@
         <v>11</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G161" s="2"/>
       <c r="H161" s="2"/>
@@ -5417,13 +5560,13 @@
         <v>11</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
@@ -5446,7 +5589,7 @@
         <v>11</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>57</v>
@@ -5475,13 +5618,13 @@
         <v>11</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
@@ -5504,13 +5647,13 @@
         <v>11</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
@@ -5533,13 +5676,13 @@
         <v>11</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
@@ -5558,14 +5701,14 @@
       <c r="B167" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>7</v>
+      <c r="C167" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>10</v>
@@ -5588,16 +5731,16 @@
         <v>70</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D168" s="10" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
@@ -5616,17 +5759,17 @@
       <c r="B169" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C169" s="5" t="s">
+      <c r="C169" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E169" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
@@ -5646,10 +5789,10 @@
         <v>70</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D170" s="10" t="s">
-        <v>67</v>
+        <v>7</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>9</v>
@@ -5677,8 +5820,8 @@
       <c r="C171" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D171" s="3" t="s">
-        <v>68</v>
+      <c r="D171" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>9</v>
@@ -5700,33 +5843,33 @@
         <f t="shared" si="3"/>
         <v>171</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C172" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E172" s="2" t="s">
+      <c r="C172" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E172" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F172" s="2" t="s">
+      <c r="F172" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G172" s="2"/>
-      <c r="H172" s="2"/>
-      <c r="I172" s="2"/>
-      <c r="J172" s="2"/>
-      <c r="K172" s="2"/>
-      <c r="L172" s="2"/>
-      <c r="M172" s="2"/>
-      <c r="N172" s="2"/>
+      <c r="G172" s="3"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="3"/>
+      <c r="K172" s="3"/>
+      <c r="L172" s="3"/>
+      <c r="M172" s="3"/>
+      <c r="N172" s="3"/>
     </row>
     <row r="173" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="17">
-        <f t="shared" ref="A173:A176" si="4">ROW() - 1</f>
+        <f t="shared" si="3"/>
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
@@ -5735,14 +5878,14 @@
       <c r="C173" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D173" s="10" t="s">
-        <v>83</v>
+      <c r="D173" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G173" s="2"/>
       <c r="H173" s="2"/>
@@ -5755,7 +5898,7 @@
     </row>
     <row r="174" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
@@ -5764,14 +5907,14 @@
       <c r="C174" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D174" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E174" s="13" t="s">
-        <v>61</v>
+      <c r="D174" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
@@ -5784,24 +5927,25 @@
     </row>
     <row r="175" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C175" s="3" t="s">
-        <v>11</v>
+      <c r="C175" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E175" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G175" s="2"/>
       <c r="H175" s="2"/>
       <c r="I175" s="2"/>
       <c r="J175" s="2"/>
@@ -5811,58 +5955,83 @@
       <c r="N175" s="2"/>
     </row>
     <row r="176" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A176" s="19">
+      <c r="A176" s="17">
+        <f t="shared" ref="A176:A180" si="4">ROW() - 1</f>
+        <v>175</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D176" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E176" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G176" s="2"/>
+      <c r="H176" s="2"/>
+      <c r="I176" s="2"/>
+      <c r="J176" s="2"/>
+      <c r="K176" s="2"/>
+      <c r="L176" s="2"/>
+      <c r="M176" s="2"/>
+      <c r="N176" s="2"/>
+    </row>
+    <row r="177" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A177" s="19">
         <f t="shared" si="4"/>
-        <v>175</v>
-      </c>
-      <c r="B176" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B177" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C176" s="20" t="s">
+      <c r="C177" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D176" s="10" t="s">
+      <c r="D177" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E176" s="13" t="s">
+      <c r="E177" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F176" s="13" t="s">
+      <c r="F177" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G176" s="13"/>
-      <c r="H176" s="13"/>
-      <c r="I176" s="13"/>
-      <c r="J176" s="13"/>
-      <c r="K176" s="13"/>
-      <c r="L176" s="13"/>
-      <c r="M176" s="13"/>
-      <c r="N176" s="13"/>
-    </row>
-    <row r="177" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A177" s="17"/>
-      <c r="B177" s="2"/>
-      <c r="C177" s="5"/>
-      <c r="D177" s="3"/>
-      <c r="E177" s="2"/>
-      <c r="F177" s="2"/>
-      <c r="G177" s="2"/>
-      <c r="H177" s="2"/>
-      <c r="I177" s="2"/>
-      <c r="J177" s="2"/>
-      <c r="K177" s="2"/>
-      <c r="L177" s="2"/>
-      <c r="M177" s="2"/>
-      <c r="N177" s="2"/>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="13"/>
+      <c r="J177" s="13"/>
+      <c r="K177" s="13"/>
+      <c r="L177" s="13"/>
+      <c r="M177" s="13"/>
+      <c r="N177" s="13"/>
     </row>
     <row r="178" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A178" s="17"/>
-      <c r="B178" s="2"/>
-      <c r="C178" s="5"/>
-      <c r="D178" s="3"/>
-      <c r="E178" s="2"/>
-      <c r="F178" s="2"/>
-      <c r="G178" s="2"/>
+      <c r="A178" s="17">
+        <f t="shared" si="4"/>
+        <v>177</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
       <c r="J178" s="2"/>
@@ -5872,12 +6041,25 @@
       <c r="N178" s="2"/>
     </row>
     <row r="179" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A179" s="17"/>
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
-      <c r="D179" s="3"/>
-      <c r="E179" s="2"/>
-      <c r="F179" s="2"/>
+      <c r="A179" s="17">
+        <f t="shared" si="3"/>
+        <v>178</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G179" s="2"/>
       <c r="H179" s="2"/>
       <c r="I179" s="2"/>
@@ -5888,12 +6070,25 @@
       <c r="N179" s="2"/>
     </row>
     <row r="180" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A180" s="17"/>
-      <c r="B180" s="2"/>
-      <c r="C180" s="5"/>
-      <c r="D180" s="3"/>
-      <c r="E180" s="2"/>
-      <c r="F180" s="2"/>
+      <c r="A180" s="17">
+        <f t="shared" si="4"/>
+        <v>179</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D180" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G180" s="2"/>
       <c r="H180" s="2"/>
       <c r="I180" s="2"/>
@@ -5938,7 +6133,7 @@
     <row r="183" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="17"/>
       <c r="B183" s="2"/>
-      <c r="C183" s="5"/>
+      <c r="C183" s="2"/>
       <c r="D183" s="3"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
@@ -5954,8 +6149,8 @@
     <row r="184" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="17"/>
       <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="3"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
@@ -5970,8 +6165,8 @@
     <row r="185" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="17"/>
       <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="3"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
@@ -5986,8 +6181,8 @@
     <row r="186" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="17"/>
       <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
-      <c r="D186" s="2"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="3"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
@@ -6002,8 +6197,8 @@
     <row r="187" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="17"/>
       <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
-      <c r="D187" s="2"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="3"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
@@ -18655,38 +18850,135 @@
       <c r="M977" s="2"/>
       <c r="N977" s="2"/>
     </row>
-    <row r="978" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="978" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A978" s="17"/>
       <c r="B978" s="2"/>
       <c r="C978" s="2"/>
       <c r="D978" s="2"/>
       <c r="E978" s="2"/>
       <c r="F978" s="2"/>
-    </row>
-    <row r="979" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G978" s="2"/>
+      <c r="H978" s="2"/>
+      <c r="I978" s="2"/>
+      <c r="J978" s="2"/>
+      <c r="K978" s="2"/>
+      <c r="L978" s="2"/>
+      <c r="M978" s="2"/>
+      <c r="N978" s="2"/>
+    </row>
+    <row r="979" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A979" s="17"/>
       <c r="B979" s="2"/>
       <c r="C979" s="2"/>
       <c r="D979" s="2"/>
       <c r="E979" s="2"/>
       <c r="F979" s="2"/>
+      <c r="G979" s="2"/>
+      <c r="H979" s="2"/>
+      <c r="I979" s="2"/>
+      <c r="J979" s="2"/>
+      <c r="K979" s="2"/>
+      <c r="L979" s="2"/>
+      <c r="M979" s="2"/>
+      <c r="N979" s="2"/>
+    </row>
+    <row r="980" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A980" s="17"/>
+      <c r="B980" s="2"/>
+      <c r="C980" s="2"/>
+      <c r="D980" s="2"/>
+      <c r="E980" s="2"/>
+      <c r="F980" s="2"/>
+      <c r="G980" s="2"/>
+      <c r="H980" s="2"/>
+      <c r="I980" s="2"/>
+      <c r="J980" s="2"/>
+      <c r="K980" s="2"/>
+      <c r="L980" s="2"/>
+      <c r="M980" s="2"/>
+      <c r="N980" s="2"/>
+    </row>
+    <row r="981" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A981" s="17"/>
+      <c r="B981" s="2"/>
+      <c r="C981" s="2"/>
+      <c r="D981" s="2"/>
+      <c r="E981" s="2"/>
+      <c r="F981" s="2"/>
+      <c r="G981" s="2"/>
+      <c r="H981" s="2"/>
+      <c r="I981" s="2"/>
+      <c r="J981" s="2"/>
+      <c r="K981" s="2"/>
+      <c r="L981" s="2"/>
+      <c r="M981" s="2"/>
+      <c r="N981" s="2"/>
+    </row>
+    <row r="982" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A982" s="17"/>
+      <c r="B982" s="2"/>
+      <c r="C982" s="2"/>
+      <c r="D982" s="2"/>
+      <c r="E982" s="2"/>
+      <c r="F982" s="2"/>
+    </row>
+    <row r="983" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A983" s="17"/>
+      <c r="B983" s="2"/>
+      <c r="C983" s="2"/>
+      <c r="D983" s="2"/>
+      <c r="E983" s="2"/>
+      <c r="F983" s="2"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A950" xr:uid="{7D54B8A3-63FE-4270-8CC6-3E45DC1F820C}"/>
+      <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F1:F979">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
+  <conditionalFormatting sqref="F171 F1:F133 F173:F983 F136:F169">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH(("No"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Write">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Write">
       <formula>NOT(ISERROR(SEARCH(("Write"),(F1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F170">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F170))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F170))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F170))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F172">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F172))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F172))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F172))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F134:F135">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F134))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F134))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F134))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18694,35 +18986,35 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B36 B177:B1048576 B38:B89 B91:B132 B134:B174</xm:sqref>
+          <xm:sqref>B1:B36 B38:B89 B179:B1048576 B91:B131 B133:B176</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$B$2:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E35 E38:E87 E177:E1048576 E91:E132 E134:E174</xm:sqref>
+          <xm:sqref>E1:E35 E38:E87 E179:E1048576 E91:E131 E133:E176</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$B$3:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D35 D38:D87 D91:D131 D177:D1048576 D134:D174</xm:sqref>
+          <xm:sqref>D1:D35 D38:D87 D91:D131 D134:D176 D179:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F35 F38:F87 F177:F1048576 F91:F132 F134:F174</xm:sqref>
+          <xm:sqref>F1:F35 F38:F87 F179:F1048576 F91:F131 F133:F176</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C35 C38:C87 C177:C1048576 C89 C91:C132 C134:C174</xm:sqref>
+          <xm:sqref>C1:C35 C38:C87 C89 C179:C1048576 C91:C131 C133:C176</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18731,13 +19023,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
@@ -19174,7 +19466,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B73">
+  <sortState ref="B4:B73">
     <sortCondition ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed Setting informations like Edit profile, Change password, Feedback Features are vanished from popups for ALSP user.
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">roles!$B$1:$B$983</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">roles!$B$1:$B$986</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="94">
   <si>
     <t>User</t>
   </si>
@@ -484,7 +484,79 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -867,10 +939,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N983"/>
+  <dimension ref="A1:N986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -941,7 +1013,7 @@
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
-        <f t="shared" ref="A3:A67" si="0">ROW() - 1</f>
+        <f t="shared" ref="A3:A70" si="0">ROW() - 1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2164,14 +2236,14 @@
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>19</v>
@@ -2193,17 +2265,17 @@
       <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2222,14 +2294,14 @@
       <c r="B47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>19</v>
@@ -2251,11 +2323,11 @@
       <c r="B48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>17</v>
@@ -2284,13 +2356,13 @@
         <v>11</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2307,19 +2379,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -2336,19 +2408,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2365,19 +2437,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2397,13 +2469,13 @@
         <v>44</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>10</v>
@@ -2422,16 +2494,16 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="13" t="s">
+      <c r="D54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
@@ -2458,10 +2530,10 @@
         <v>11</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>10</v>
@@ -2486,11 +2558,11 @@
       <c r="C56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>8</v>
+      <c r="D56" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>10</v>
@@ -2509,20 +2581,20 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -2545,13 +2617,13 @@
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -2574,13 +2646,13 @@
         <v>11</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -2600,13 +2672,13 @@
         <v>44</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>19</v>
@@ -2632,7 +2704,7 @@
         <v>11</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>17</v>
@@ -2661,7 +2733,7 @@
         <v>11</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>17</v>
@@ -2690,7 +2762,7 @@
         <v>11</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>17</v>
@@ -2719,7 +2791,7 @@
         <v>11</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>17</v>
@@ -2745,16 +2817,16 @@
         <v>44</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -2774,16 +2846,16 @@
         <v>44</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -2806,10 +2878,10 @@
         <v>11</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>19</v>
@@ -2825,23 +2897,23 @@
     </row>
     <row r="68" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
-        <f t="shared" ref="A68:A104" si="1">ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>11</v>
+      <c r="C68" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -2854,23 +2926,23 @@
     </row>
     <row r="69" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>11</v>
+      <c r="C69" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -2883,23 +2955,23 @@
     </row>
     <row r="70" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2912,23 +2984,23 @@
     </row>
     <row r="71" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A71:A107" si="1">ROW() - 1</f>
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2947,14 +3019,14 @@
       <c r="B72" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>19</v>
@@ -2977,13 +3049,13 @@
         <v>44</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>10</v>
@@ -3006,16 +3078,16 @@
         <v>44</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -3034,14 +3106,14 @@
       <c r="B75" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>19</v>
@@ -3063,17 +3135,17 @@
       <c r="B76" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -3092,14 +3164,14 @@
       <c r="B77" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>11</v>
+      <c r="C77" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>19</v>
@@ -3122,13 +3194,13 @@
         <v>44</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>19</v>
@@ -3154,13 +3226,13 @@
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3183,13 +3255,13 @@
         <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3209,13 +3281,13 @@
         <v>44</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>19</v>
@@ -3241,10 +3313,10 @@
         <v>11</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>10</v>
@@ -3270,10 +3342,10 @@
         <v>11</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>10</v>
@@ -3298,14 +3370,14 @@
       <c r="C84" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D84" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>33</v>
+      <c r="D84" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -3328,7 +3400,7 @@
         <v>11</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>35</v>
@@ -3357,10 +3429,10 @@
         <v>11</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>10</v>
@@ -3383,16 +3455,16 @@
         <v>44</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -3411,14 +3483,14 @@
       <c r="B88" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>10</v>
@@ -3434,19 +3506,20 @@
     </row>
     <row r="89" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
-        <v>87</v>
+        <f t="shared" si="1"/>
+        <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>10</v>
@@ -3461,47 +3534,47 @@
       <c r="N89" s="2"/>
     </row>
     <row r="90" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A90" s="19">
-        <f t="shared" ref="A90" si="2">ROW() - 1</f>
+      <c r="A90" s="17">
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C90" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F90" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13"/>
-      <c r="N90" s="13"/>
+      <c r="C90" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
     </row>
     <row r="91" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>9</v>
@@ -3520,23 +3593,22 @@
     </row>
     <row r="92" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
-        <f t="shared" si="1"/>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C92" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -3548,53 +3620,53 @@
       <c r="N92" s="2"/>
     </row>
     <row r="93" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="17">
-        <f t="shared" si="1"/>
+      <c r="A93" s="19">
+        <f t="shared" ref="A93" si="2">ROW() - 1</f>
         <v>92</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C93" s="2" t="s">
+      <c r="B93" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="2"/>
-      <c r="N93" s="2"/>
+      <c r="D93" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="13"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="13"/>
+      <c r="M93" s="13"/>
+      <c r="N93" s="13"/>
     </row>
     <row r="94" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
-        <f t="shared" si="1"/>
+        <f>ROW() - 1</f>
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -3614,13 +3686,13 @@
         <v>49</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>19</v>
@@ -3646,7 +3718,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>17</v>
@@ -3675,7 +3747,7 @@
         <v>11</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>17</v>
@@ -3704,7 +3776,7 @@
         <v>11</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>17</v>
@@ -3733,7 +3805,7 @@
         <v>11</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>17</v>
@@ -3759,13 +3831,13 @@
         <v>49</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>19</v>
@@ -3788,13 +3860,13 @@
         <v>49</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>88</v>
+        <v>11</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>19</v>
@@ -3817,13 +3889,13 @@
         <v>49</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>19</v>
@@ -3849,7 +3921,7 @@
         <v>7</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>9</v>
@@ -3875,13 +3947,13 @@
         <v>49</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="D104" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>19</v>
@@ -3897,20 +3969,20 @@
     </row>
     <row r="105" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
-        <f>ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>19</v>
@@ -3926,20 +3998,20 @@
     </row>
     <row r="106" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
-        <f t="shared" ref="A106:A179" si="3">ROW() - 1</f>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>19</v>
@@ -3955,17 +4027,17 @@
     </row>
     <row r="107" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C107" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>51</v>
@@ -3984,17 +4056,17 @@
     </row>
     <row r="108" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
-        <f t="shared" si="3"/>
+        <f>ROW() - 1</f>
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C108" s="5" t="s">
+      <c r="C108" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>51</v>
@@ -4013,23 +4085,23 @@
     </row>
     <row r="109" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A109:A182" si="3">ROW() - 1</f>
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -4048,17 +4120,17 @@
       <c r="B110" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>7</v>
+      <c r="C110" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
@@ -4081,10 +4153,10 @@
         <v>11</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>19</v>
@@ -4106,17 +4178,17 @@
       <c r="B112" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C112" s="5" t="s">
-        <v>11</v>
+      <c r="C112" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
@@ -4135,17 +4207,17 @@
       <c r="B113" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C113" s="5" t="s">
-        <v>11</v>
+      <c r="C113" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -4165,16 +4237,16 @@
         <v>49</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
@@ -4197,13 +4269,13 @@
         <v>11</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
@@ -4226,13 +4298,13 @@
         <v>11</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
@@ -4252,16 +4324,16 @@
         <v>49</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
@@ -4284,13 +4356,13 @@
         <v>11</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
@@ -4313,7 +4385,7 @@
         <v>11</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>57</v>
@@ -4342,7 +4414,7 @@
         <v>11</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>57</v>
@@ -4371,7 +4443,7 @@
         <v>11</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>57</v>
@@ -4400,7 +4472,7 @@
         <v>11</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>57</v>
@@ -4429,13 +4501,13 @@
         <v>11</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
@@ -4454,17 +4526,17 @@
       <c r="B124" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>7</v>
+      <c r="C124" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
@@ -4484,16 +4556,16 @@
         <v>49</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
@@ -4516,13 +4588,13 @@
         <v>11</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
@@ -4538,29 +4610,29 @@
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D127" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E127" s="3" t="s">
+      <c r="D127" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F127" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G127" s="3"/>
-      <c r="H127" s="3"/>
-      <c r="I127" s="3"/>
-      <c r="J127" s="3"/>
-      <c r="K127" s="3"/>
-      <c r="L127" s="3"/>
-      <c r="M127" s="3"/>
-      <c r="N127" s="3"/>
+      <c r="F127" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+      <c r="L127" s="2"/>
+      <c r="M127" s="2"/>
+      <c r="N127" s="2"/>
     </row>
     <row r="128" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
@@ -4571,10 +4643,10 @@
         <v>49</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>9</v>
@@ -4603,7 +4675,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>9</v>
@@ -4611,43 +4683,43 @@
       <c r="F129" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G129" s="3"/>
-      <c r="H129" s="3"/>
-      <c r="I129" s="3"/>
-      <c r="J129" s="3"/>
-      <c r="K129" s="3"/>
-      <c r="L129" s="3"/>
-      <c r="M129" s="3"/>
-      <c r="N129" s="3"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2"/>
+      <c r="K129" s="2"/>
+      <c r="L129" s="2"/>
+      <c r="M129" s="2"/>
+      <c r="N129" s="2"/>
     </row>
     <row r="130" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="17">
         <f t="shared" si="3"/>
         <v>129</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C130" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D130" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E130" s="2" t="s">
+      <c r="D130" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E130" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="F130" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
-      <c r="I130" s="2"/>
-      <c r="J130" s="2"/>
-      <c r="K130" s="2"/>
-      <c r="L130" s="2"/>
-      <c r="M130" s="2"/>
-      <c r="N130" s="2"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3"/>
+      <c r="M130" s="3"/>
+      <c r="N130" s="3"/>
     </row>
     <row r="131" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="17">
@@ -4660,52 +4732,52 @@
       <c r="C131" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D131" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E131" s="13" t="s">
-        <v>61</v>
+      <c r="D131" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G131" s="3"/>
-      <c r="H131" s="3"/>
-      <c r="I131" s="3"/>
-      <c r="J131" s="3"/>
-      <c r="K131" s="3"/>
-      <c r="L131" s="3"/>
-      <c r="M131" s="3"/>
-      <c r="N131" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+      <c r="L131" s="2"/>
+      <c r="M131" s="2"/>
+      <c r="N131" s="2"/>
     </row>
     <row r="132" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A132" s="19">
+      <c r="A132" s="17">
         <f t="shared" si="3"/>
         <v>131</v>
       </c>
-      <c r="B132" s="13" t="s">
+      <c r="B132" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C132" s="20" t="s">
+      <c r="C132" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D132" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E132" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F132" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G132" s="13"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
-      <c r="J132" s="13"/>
-      <c r="K132" s="13"/>
-      <c r="L132" s="13"/>
-      <c r="M132" s="13"/>
-      <c r="N132" s="13"/>
+      <c r="D132" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="3"/>
+      <c r="N132" s="3"/>
     </row>
     <row r="133" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="17">
@@ -4715,26 +4787,26 @@
       <c r="B133" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>11</v>
+      <c r="C133" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G133" s="3"/>
-      <c r="H133" s="3"/>
-      <c r="I133" s="3"/>
-      <c r="J133" s="3"/>
-      <c r="K133" s="3"/>
-      <c r="L133" s="3"/>
-      <c r="M133" s="3"/>
-      <c r="N133" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2"/>
+      <c r="K133" s="2"/>
+      <c r="L133" s="2"/>
+      <c r="M133" s="2"/>
+      <c r="N133" s="2"/>
     </row>
     <row r="134" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="17">
@@ -4745,54 +4817,54 @@
         <v>49</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D134" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E134" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
-      <c r="J134" s="2"/>
-      <c r="K134" s="2"/>
-      <c r="L134" s="2"/>
-      <c r="M134" s="2"/>
-      <c r="N134" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
+      <c r="M134" s="3"/>
+      <c r="N134" s="3"/>
     </row>
     <row r="135" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A135" s="17">
+      <c r="A135" s="19">
         <f t="shared" si="3"/>
         <v>134</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="C135" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D135" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F135" s="2" t="s">
+      <c r="D135" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E135" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F135" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-      <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-      <c r="K135" s="2"/>
-      <c r="L135" s="2"/>
-      <c r="M135" s="2"/>
-      <c r="N135" s="2"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="13"/>
+      <c r="K135" s="13"/>
+      <c r="L135" s="13"/>
+      <c r="M135" s="13"/>
+      <c r="N135" s="13"/>
     </row>
     <row r="136" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="17">
@@ -4800,13 +4872,13 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>9</v>
@@ -4829,13 +4901,13 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C137" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C137" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>9</v>
@@ -4843,14 +4915,14 @@
       <c r="F137" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G137" s="3"/>
-      <c r="H137" s="3"/>
-      <c r="I137" s="3"/>
-      <c r="J137" s="3"/>
-      <c r="K137" s="3"/>
-      <c r="L137" s="3"/>
-      <c r="M137" s="3"/>
-      <c r="N137" s="3"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+      <c r="L137" s="2"/>
+      <c r="M137" s="2"/>
+      <c r="N137" s="2"/>
     </row>
     <row r="138" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
@@ -4858,28 +4930,28 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C138" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C138" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>18</v>
+      <c r="D138" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G138" s="3"/>
-      <c r="H138" s="3"/>
-      <c r="I138" s="3"/>
-      <c r="J138" s="3"/>
-      <c r="K138" s="3"/>
-      <c r="L138" s="3"/>
-      <c r="M138" s="3"/>
-      <c r="N138" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2"/>
+      <c r="K138" s="2"/>
+      <c r="L138" s="2"/>
+      <c r="M138" s="2"/>
+      <c r="N138" s="2"/>
     </row>
     <row r="139" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="17">
@@ -4890,16 +4962,16 @@
         <v>70</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D139" s="10" t="s">
-        <v>84</v>
+        <v>7</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
@@ -4919,13 +4991,13 @@
         <v>70</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>19</v>
@@ -4951,7 +5023,7 @@
         <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>17</v>
@@ -4979,8 +5051,8 @@
       <c r="C142" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D142" s="3" t="s">
-        <v>22</v>
+      <c r="D142" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>17</v>
@@ -5009,7 +5081,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>17</v>
@@ -5038,7 +5110,7 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>17</v>
@@ -5064,25 +5136,25 @@
         <v>70</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
-      <c r="J145" s="2"/>
-      <c r="K145" s="2"/>
-      <c r="L145" s="2"/>
-      <c r="M145" s="2"/>
-      <c r="N145" s="2"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3"/>
     </row>
     <row r="146" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
@@ -5093,16 +5165,16 @@
         <v>70</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
@@ -5122,25 +5194,25 @@
         <v>70</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="2"/>
-      <c r="L147" s="2"/>
-      <c r="M147" s="2"/>
-      <c r="N147" s="2"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="3"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
     </row>
     <row r="148" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="17">
@@ -5154,7 +5226,7 @@
         <v>7</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>9</v>
@@ -5162,14 +5234,14 @@
       <c r="F148" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G148" s="3"/>
-      <c r="H148" s="3"/>
-      <c r="I148" s="3"/>
-      <c r="J148" s="3"/>
-      <c r="K148" s="3"/>
-      <c r="L148" s="3"/>
-      <c r="M148" s="3"/>
-      <c r="N148" s="3"/>
+      <c r="G148" s="2"/>
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2"/>
+      <c r="K148" s="2"/>
+      <c r="L148" s="2"/>
+      <c r="M148" s="2"/>
+      <c r="N148" s="2"/>
     </row>
     <row r="149" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="17">
@@ -5180,16 +5252,16 @@
         <v>70</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
@@ -5209,25 +5281,25 @@
         <v>70</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G150" s="3"/>
-      <c r="H150" s="3"/>
-      <c r="I150" s="3"/>
-      <c r="J150" s="3"/>
-      <c r="K150" s="3"/>
-      <c r="L150" s="3"/>
-      <c r="M150" s="3"/>
-      <c r="N150" s="3"/>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+      <c r="J150" s="2"/>
+      <c r="K150" s="2"/>
+      <c r="L150" s="2"/>
+      <c r="M150" s="2"/>
+      <c r="N150" s="2"/>
     </row>
     <row r="151" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="17">
@@ -5238,13 +5310,13 @@
         <v>70</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>19</v>
@@ -5266,11 +5338,11 @@
       <c r="B152" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C152" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>51</v>
@@ -5295,11 +5367,11 @@
       <c r="B153" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C153" s="5" t="s">
+      <c r="C153" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>51</v>
@@ -5325,16 +5397,16 @@
         <v>70</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
@@ -5353,17 +5425,17 @@
       <c r="B155" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>7</v>
+      <c r="C155" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
@@ -5386,10 +5458,10 @@
         <v>11</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>19</v>
@@ -5411,17 +5483,17 @@
       <c r="B157" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C157" s="5" t="s">
-        <v>11</v>
+      <c r="C157" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
@@ -5440,17 +5512,17 @@
       <c r="B158" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C158" s="5" t="s">
-        <v>11</v>
+      <c r="C158" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
@@ -5470,16 +5542,16 @@
         <v>70</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
@@ -5502,13 +5574,13 @@
         <v>11</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
@@ -5531,22 +5603,22 @@
         <v>11</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-      <c r="I161" s="2"/>
-      <c r="J161" s="2"/>
-      <c r="K161" s="2"/>
-      <c r="L161" s="2"/>
-      <c r="M161" s="2"/>
-      <c r="N161" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="G161" s="3"/>
+      <c r="H161" s="3"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="3"/>
+      <c r="K161" s="3"/>
+      <c r="L161" s="3"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
     </row>
     <row r="162" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="17">
@@ -5557,25 +5629,25 @@
         <v>70</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
-      <c r="I162" s="2"/>
-      <c r="J162" s="2"/>
-      <c r="K162" s="2"/>
-      <c r="L162" s="2"/>
-      <c r="M162" s="2"/>
-      <c r="N162" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G162" s="3"/>
+      <c r="H162" s="3"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="3"/>
+      <c r="K162" s="3"/>
+      <c r="L162" s="3"/>
+      <c r="M162" s="3"/>
+      <c r="N162" s="3"/>
     </row>
     <row r="163" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="17">
@@ -5589,22 +5661,22 @@
         <v>11</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
-      <c r="I163" s="2"/>
-      <c r="J163" s="2"/>
-      <c r="K163" s="2"/>
-      <c r="L163" s="2"/>
-      <c r="M163" s="2"/>
-      <c r="N163" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G163" s="3"/>
+      <c r="H163" s="3"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
     </row>
     <row r="164" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="17">
@@ -5618,7 +5690,7 @@
         <v>11</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>57</v>
@@ -5647,7 +5719,7 @@
         <v>11</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>57</v>
@@ -5676,7 +5748,7 @@
         <v>11</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>57</v>
@@ -5705,7 +5777,7 @@
         <v>11</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>57</v>
@@ -5734,13 +5806,13 @@
         <v>11</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
@@ -5759,17 +5831,17 @@
       <c r="B169" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C169" s="2" t="s">
-        <v>7</v>
+      <c r="C169" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
@@ -5789,16 +5861,16 @@
         <v>70</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
@@ -5820,14 +5892,14 @@
       <c r="C171" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D171" s="10" t="s">
-        <v>67</v>
+      <c r="D171" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G171" s="2"/>
       <c r="H171" s="2"/>
@@ -5843,29 +5915,29 @@
         <f t="shared" si="3"/>
         <v>171</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B172" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C172" s="3" t="s">
+      <c r="C172" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D172" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E172" s="3" t="s">
+      <c r="D172" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E172" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F172" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G172" s="3"/>
-      <c r="H172" s="3"/>
-      <c r="I172" s="3"/>
-      <c r="J172" s="3"/>
-      <c r="K172" s="3"/>
-      <c r="L172" s="3"/>
-      <c r="M172" s="3"/>
-      <c r="N172" s="3"/>
+      <c r="F172" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G172" s="2"/>
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
+      <c r="J172" s="2"/>
+      <c r="K172" s="2"/>
+      <c r="L172" s="2"/>
+      <c r="M172" s="2"/>
+      <c r="N172" s="2"/>
     </row>
     <row r="173" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="17">
@@ -5876,10 +5948,10 @@
         <v>70</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>9</v>
@@ -5907,8 +5979,8 @@
       <c r="C174" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D174" s="3" t="s">
-        <v>69</v>
+      <c r="D174" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>9</v>
@@ -5930,33 +6002,33 @@
         <f t="shared" si="3"/>
         <v>174</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C175" s="5" t="s">
+      <c r="C175" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E175" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E175" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F175" s="2" t="s">
+      <c r="F175" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G175" s="2"/>
-      <c r="H175" s="2"/>
-      <c r="I175" s="2"/>
-      <c r="J175" s="2"/>
-      <c r="K175" s="2"/>
-      <c r="L175" s="2"/>
-      <c r="M175" s="2"/>
-      <c r="N175" s="2"/>
+      <c r="G175" s="3"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="3"/>
+      <c r="K175" s="3"/>
+      <c r="L175" s="3"/>
+      <c r="M175" s="3"/>
+      <c r="N175" s="3"/>
     </row>
     <row r="176" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="17">
-        <f t="shared" ref="A176:A180" si="4">ROW() - 1</f>
+        <f t="shared" si="3"/>
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
@@ -5965,14 +6037,14 @@
       <c r="C176" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D176" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E176" s="13" t="s">
-        <v>61</v>
+      <c r="D176" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G176" s="2"/>
       <c r="H176" s="2"/>
@@ -5984,54 +6056,55 @@
       <c r="N176" s="2"/>
     </row>
     <row r="177" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A177" s="19">
-        <f t="shared" si="4"/>
+      <c r="A177" s="17">
+        <f t="shared" si="3"/>
         <v>176</v>
       </c>
-      <c r="B177" s="13" t="s">
+      <c r="B177" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C177" s="20" t="s">
+      <c r="C177" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D177" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E177" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F177" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G177" s="13"/>
-      <c r="H177" s="13"/>
-      <c r="I177" s="13"/>
-      <c r="J177" s="13"/>
-      <c r="K177" s="13"/>
-      <c r="L177" s="13"/>
-      <c r="M177" s="13"/>
-      <c r="N177" s="13"/>
+      <c r="D177" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G177" s="2"/>
+      <c r="H177" s="2"/>
+      <c r="I177" s="2"/>
+      <c r="J177" s="2"/>
+      <c r="K177" s="2"/>
+      <c r="L177" s="2"/>
+      <c r="M177" s="2"/>
+      <c r="N177" s="2"/>
     </row>
     <row r="178" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C178" s="3" t="s">
-        <v>11</v>
+      <c r="C178" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E178" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G178" s="2"/>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
       <c r="J178" s="2"/>
@@ -6042,23 +6115,23 @@
     </row>
     <row r="179" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A179:A183" si="4">ROW() - 1</f>
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D179" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E179" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G179" s="2"/>
       <c r="H179" s="2"/>
@@ -6070,42 +6143,54 @@
       <c r="N179" s="2"/>
     </row>
     <row r="180" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A180" s="17">
+      <c r="A180" s="19">
         <f t="shared" si="4"/>
         <v>179</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C180" s="5" t="s">
+      <c r="C180" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E180" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F180" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E180" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F180" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G180" s="2"/>
-      <c r="H180" s="2"/>
-      <c r="I180" s="2"/>
-      <c r="J180" s="2"/>
-      <c r="K180" s="2"/>
-      <c r="L180" s="2"/>
-      <c r="M180" s="2"/>
-      <c r="N180" s="2"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="13"/>
+      <c r="K180" s="13"/>
+      <c r="L180" s="13"/>
+      <c r="M180" s="13"/>
+      <c r="N180" s="13"/>
     </row>
     <row r="181" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A181" s="17"/>
-      <c r="B181" s="2"/>
-      <c r="C181" s="5"/>
-      <c r="D181" s="3"/>
-      <c r="E181" s="2"/>
-      <c r="F181" s="2"/>
-      <c r="G181" s="2"/>
+      <c r="A181" s="17">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D181" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
       <c r="J181" s="2"/>
@@ -6115,12 +6200,25 @@
       <c r="N181" s="2"/>
     </row>
     <row r="182" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A182" s="17"/>
-      <c r="B182" s="2"/>
-      <c r="C182" s="5"/>
-      <c r="D182" s="3"/>
-      <c r="E182" s="2"/>
-      <c r="F182" s="2"/>
+      <c r="A182" s="17">
+        <f t="shared" si="3"/>
+        <v>181</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
@@ -6131,12 +6229,25 @@
       <c r="N182" s="2"/>
     </row>
     <row r="183" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A183" s="17"/>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
-      <c r="D183" s="3"/>
-      <c r="E183" s="2"/>
-      <c r="F183" s="2"/>
+      <c r="A183" s="17">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D183" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
@@ -6181,7 +6292,7 @@
     <row r="186" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="17"/>
       <c r="B186" s="2"/>
-      <c r="C186" s="5"/>
+      <c r="C186" s="2"/>
       <c r="D186" s="3"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
@@ -6213,8 +6324,8 @@
     <row r="188" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="17"/>
       <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
-      <c r="D188" s="2"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="3"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
@@ -6229,8 +6340,8 @@
     <row r="189" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="17"/>
       <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
-      <c r="D189" s="2"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="3"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
@@ -6245,8 +6356,8 @@
     <row r="190" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="17"/>
       <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
-      <c r="D190" s="2"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="3"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
@@ -18914,21 +19025,69 @@
       <c r="M981" s="2"/>
       <c r="N981" s="2"/>
     </row>
-    <row r="982" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="982" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A982" s="17"/>
       <c r="B982" s="2"/>
       <c r="C982" s="2"/>
       <c r="D982" s="2"/>
       <c r="E982" s="2"/>
       <c r="F982" s="2"/>
-    </row>
-    <row r="983" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G982" s="2"/>
+      <c r="H982" s="2"/>
+      <c r="I982" s="2"/>
+      <c r="J982" s="2"/>
+      <c r="K982" s="2"/>
+      <c r="L982" s="2"/>
+      <c r="M982" s="2"/>
+      <c r="N982" s="2"/>
+    </row>
+    <row r="983" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A983" s="17"/>
       <c r="B983" s="2"/>
       <c r="C983" s="2"/>
       <c r="D983" s="2"/>
       <c r="E983" s="2"/>
       <c r="F983" s="2"/>
+      <c r="G983" s="2"/>
+      <c r="H983" s="2"/>
+      <c r="I983" s="2"/>
+      <c r="J983" s="2"/>
+      <c r="K983" s="2"/>
+      <c r="L983" s="2"/>
+      <c r="M983" s="2"/>
+      <c r="N983" s="2"/>
+    </row>
+    <row r="984" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A984" s="17"/>
+      <c r="B984" s="2"/>
+      <c r="C984" s="2"/>
+      <c r="D984" s="2"/>
+      <c r="E984" s="2"/>
+      <c r="F984" s="2"/>
+      <c r="G984" s="2"/>
+      <c r="H984" s="2"/>
+      <c r="I984" s="2"/>
+      <c r="J984" s="2"/>
+      <c r="K984" s="2"/>
+      <c r="L984" s="2"/>
+      <c r="M984" s="2"/>
+      <c r="N984" s="2"/>
+    </row>
+    <row r="985" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A985" s="17"/>
+      <c r="B985" s="2"/>
+      <c r="C985" s="2"/>
+      <c r="D985" s="2"/>
+      <c r="E985" s="2"/>
+      <c r="F985" s="2"/>
+    </row>
+    <row r="986" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A986" s="17"/>
+      <c r="B986" s="2"/>
+      <c r="C986" s="2"/>
+      <c r="D986" s="2"/>
+      <c r="E986" s="2"/>
+      <c r="F986" s="2"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -18937,48 +19096,81 @@
       <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F171 F1:F133 F173:F983 F136:F169">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Read">
+  <conditionalFormatting sqref="F174 F1:F44 F176:F986 F139:F172 F48:F136">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH(("No"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Write">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Write">
       <formula>NOT(ISERROR(SEARCH(("Write"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170">
+  <conditionalFormatting sqref="F173">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F173))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F173))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F173))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F175">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F175))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F175))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F175))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F137:F138">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Read">
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F137))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH(("No"),(F137))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Write">
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F137))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45">
     <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F170))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F45))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F170))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("No"),(F45))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F170))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F45))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F172">
+  <conditionalFormatting sqref="F46">
     <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F172))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F46))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F172))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("No"),(F46))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F172))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F46))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F134:F135">
+  <conditionalFormatting sqref="F47">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F134))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Read"),(F47))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F134))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("No"),(F47))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F134))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Write"),(F47))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18990,31 +19182,31 @@
           <x14:formula1>
             <xm:f>ScreenIds!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B36 B38:B89 B179:B1048576 B91:B131 B133:B176</xm:sqref>
+          <xm:sqref>B1:B36 B136:B179 B182:B1048576 B94:B134 B38:B92</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$B$2:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E35 E38:E87 E179:E1048576 E91:E131 E133:E176</xm:sqref>
+          <xm:sqref>E1:E35 E136:E179 E182:E1048576 E94:E134 E38:E90</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$B$3:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D35 D38:D87 D91:D131 D134:D176 D179:D1048576</xm:sqref>
+          <xm:sqref>D1:D35 D182:D1048576 D94:D134 D137:D179 D38:D90</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F35 F38:F87 F179:F1048576 F91:F131 F133:F176</xm:sqref>
+          <xm:sqref>F1:F35 F136:F179 F182:F1048576 F94:F134 F38:F90</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ScreenIds!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C35 C38:C87 C89 C179:C1048576 C91:C131 C133:C176</xm:sqref>
+          <xm:sqref>C1:C35 C136:C179 C92 C182:C1048576 C94:C134 C38:C90</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
User Managm Permissions for Admin, Platform Admin
</commit_message>
<xml_diff>
--- a/permissions.xlsx
+++ b/permissions.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\permissions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFD3E41-8879-4BDD-AF12-D17C4A164C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="1" r:id="rId1"/>
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">roles!$B$1:$B$986</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">roles!$B$1:$B$990</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{49968090-594F-4035-ABCC-088176AC5527}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="94">
   <si>
     <t>User</t>
   </si>
@@ -326,7 +327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -484,223 +485,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -935,14 +720,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N986"/>
+  <dimension ref="A1:N990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E191" sqref="E191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4085,7 +3870,7 @@
     </row>
     <row r="109" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
-        <f t="shared" ref="A109:A182" si="3">ROW() - 1</f>
+        <f t="shared" ref="A109:A188" si="3">ROW() - 1</f>
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -4959,28 +4744,28 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G139" s="3"/>
-      <c r="H139" s="3"/>
-      <c r="I139" s="3"/>
-      <c r="J139" s="3"/>
-      <c r="K139" s="3"/>
-      <c r="L139" s="3"/>
-      <c r="M139" s="3"/>
-      <c r="N139" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+      <c r="L139" s="2"/>
+      <c r="M139" s="2"/>
+      <c r="N139" s="2"/>
     </row>
     <row r="140" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="17">
@@ -4988,28 +4773,28 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G140" s="3"/>
-      <c r="H140" s="3"/>
-      <c r="I140" s="3"/>
-      <c r="J140" s="3"/>
-      <c r="K140" s="3"/>
-      <c r="L140" s="3"/>
-      <c r="M140" s="3"/>
-      <c r="N140" s="3"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
     </row>
     <row r="141" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="17">
@@ -5017,28 +4802,28 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C141" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C141" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G141" s="3"/>
-      <c r="H141" s="3"/>
-      <c r="I141" s="3"/>
-      <c r="J141" s="3"/>
-      <c r="K141" s="3"/>
-      <c r="L141" s="3"/>
-      <c r="M141" s="3"/>
-      <c r="N141" s="3"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+      <c r="L141" s="2"/>
+      <c r="M141" s="2"/>
+      <c r="N141" s="2"/>
     </row>
     <row r="142" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="17">
@@ -5046,28 +4831,28 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C142" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C142" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D142" s="10" t="s">
-        <v>84</v>
+      <c r="D142" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G142" s="3"/>
-      <c r="H142" s="3"/>
-      <c r="I142" s="3"/>
-      <c r="J142" s="3"/>
-      <c r="K142" s="3"/>
-      <c r="L142" s="3"/>
-      <c r="M142" s="3"/>
-      <c r="N142" s="3"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2"/>
+      <c r="K142" s="2"/>
+      <c r="L142" s="2"/>
+      <c r="M142" s="2"/>
+      <c r="N142" s="2"/>
     </row>
     <row r="143" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="17">
@@ -5078,16 +4863,16 @@
         <v>70</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
@@ -5107,13 +4892,13 @@
         <v>70</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>19</v>
@@ -5139,7 +4924,7 @@
         <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>17</v>
@@ -5167,8 +4952,8 @@
       <c r="C146" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D146" s="3" t="s">
-        <v>23</v>
+      <c r="D146" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>17</v>
@@ -5197,7 +4982,7 @@
         <v>11</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>17</v>
@@ -5223,25 +5008,25 @@
         <v>70</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-      <c r="L148" s="2"/>
-      <c r="M148" s="2"/>
-      <c r="N148" s="2"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
     </row>
     <row r="149" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="17">
@@ -5252,16 +5037,16 @@
         <v>70</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
@@ -5281,25 +5066,25 @@
         <v>70</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
-      <c r="J150" s="2"/>
-      <c r="K150" s="2"/>
-      <c r="L150" s="2"/>
-      <c r="M150" s="2"/>
-      <c r="N150" s="2"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="3"/>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3"/>
     </row>
     <row r="151" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="17">
@@ -5310,13 +5095,13 @@
         <v>70</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>19</v>
@@ -5339,25 +5124,25 @@
         <v>70</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G152" s="3"/>
-      <c r="H152" s="3"/>
-      <c r="I152" s="3"/>
-      <c r="J152" s="3"/>
-      <c r="K152" s="3"/>
-      <c r="L152" s="3"/>
-      <c r="M152" s="3"/>
-      <c r="N152" s="3"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="2"/>
+      <c r="L152" s="2"/>
+      <c r="M152" s="2"/>
+      <c r="N152" s="2"/>
     </row>
     <row r="153" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="17">
@@ -5368,16 +5153,16 @@
         <v>70</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
@@ -5397,25 +5182,25 @@
         <v>70</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G154" s="3"/>
-      <c r="H154" s="3"/>
-      <c r="I154" s="3"/>
-      <c r="J154" s="3"/>
-      <c r="K154" s="3"/>
-      <c r="L154" s="3"/>
-      <c r="M154" s="3"/>
-      <c r="N154" s="3"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
+      <c r="L154" s="2"/>
+      <c r="M154" s="2"/>
+      <c r="N154" s="2"/>
     </row>
     <row r="155" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="17">
@@ -5425,14 +5210,14 @@
       <c r="B155" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C155" s="5" t="s">
-        <v>11</v>
+      <c r="C155" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>19</v>
@@ -5454,11 +5239,11 @@
       <c r="B156" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C156" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>51</v>
@@ -5484,16 +5269,16 @@
         <v>70</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
@@ -5513,16 +5298,16 @@
         <v>70</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
@@ -5545,10 +5330,10 @@
         <v>11</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>19</v>
@@ -5574,10 +5359,10 @@
         <v>11</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>19</v>
@@ -5599,17 +5384,17 @@
       <c r="B161" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C161" s="5" t="s">
-        <v>11</v>
+      <c r="C161" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
@@ -5628,14 +5413,14 @@
       <c r="B162" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C162" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>10</v>
@@ -5661,13 +5446,13 @@
         <v>11</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
@@ -5690,22 +5475,22 @@
         <v>11</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
-      <c r="I164" s="2"/>
-      <c r="J164" s="2"/>
-      <c r="K164" s="2"/>
-      <c r="L164" s="2"/>
-      <c r="M164" s="2"/>
-      <c r="N164" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="G164" s="3"/>
+      <c r="H164" s="3"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="3"/>
+      <c r="K164" s="3"/>
+      <c r="L164" s="3"/>
+      <c r="M164" s="3"/>
+      <c r="N164" s="3"/>
     </row>
     <row r="165" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="17">
@@ -5719,22 +5504,22 @@
         <v>11</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
-      <c r="I165" s="2"/>
-      <c r="J165" s="2"/>
-      <c r="K165" s="2"/>
-      <c r="L165" s="2"/>
-      <c r="M165" s="2"/>
-      <c r="N165" s="2"/>
+      <c r="G165" s="3"/>
+      <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="3"/>
+      <c r="K165" s="3"/>
+      <c r="L165" s="3"/>
+      <c r="M165" s="3"/>
+      <c r="N165" s="3"/>
     </row>
     <row r="166" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="17">
@@ -5745,25 +5530,25 @@
         <v>70</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G166" s="2"/>
-      <c r="H166" s="2"/>
-      <c r="I166" s="2"/>
-      <c r="J166" s="2"/>
-      <c r="K166" s="2"/>
-      <c r="L166" s="2"/>
-      <c r="M166" s="2"/>
-      <c r="N166" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G166" s="3"/>
+      <c r="H166" s="3"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+      <c r="L166" s="3"/>
+      <c r="M166" s="3"/>
+      <c r="N166" s="3"/>
     </row>
     <row r="167" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="17">
@@ -5777,7 +5562,7 @@
         <v>11</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>57</v>
@@ -5785,14 +5570,14 @@
       <c r="F167" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="I167" s="2"/>
-      <c r="J167" s="2"/>
-      <c r="K167" s="2"/>
-      <c r="L167" s="2"/>
-      <c r="M167" s="2"/>
-      <c r="N167" s="2"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="3"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="3"/>
+      <c r="K167" s="3"/>
+      <c r="L167" s="3"/>
+      <c r="M167" s="3"/>
+      <c r="N167" s="3"/>
     </row>
     <row r="168" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="17">
@@ -5806,13 +5591,13 @@
         <v>11</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
@@ -5835,7 +5620,7 @@
         <v>11</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E169" s="2" t="s">
         <v>57</v>
@@ -5864,13 +5649,13 @@
         <v>11</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
@@ -5893,7 +5678,7 @@
         <v>11</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>57</v>
@@ -5918,17 +5703,17 @@
       <c r="B172" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>7</v>
+      <c r="C172" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
@@ -5948,13 +5733,13 @@
         <v>70</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>19</v>
@@ -5979,14 +5764,14 @@
       <c r="C174" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D174" s="10" t="s">
-        <v>67</v>
+      <c r="D174" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
@@ -6002,29 +5787,29 @@
         <f t="shared" si="3"/>
         <v>174</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B175" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C175" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D175" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F175" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G175" s="3"/>
-      <c r="H175" s="3"/>
-      <c r="I175" s="3"/>
-      <c r="J175" s="3"/>
-      <c r="K175" s="3"/>
-      <c r="L175" s="3"/>
-      <c r="M175" s="3"/>
-      <c r="N175" s="3"/>
+      <c r="C175" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G175" s="2"/>
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+      <c r="J175" s="2"/>
+      <c r="K175" s="2"/>
+      <c r="L175" s="2"/>
+      <c r="M175" s="2"/>
+      <c r="N175" s="2"/>
     </row>
     <row r="176" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="17">
@@ -6034,17 +5819,17 @@
       <c r="B176" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C176" s="5" t="s">
-        <v>11</v>
+      <c r="C176" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E176" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G176" s="2"/>
       <c r="H176" s="2"/>
@@ -6064,10 +5849,10 @@
         <v>70</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="E177" s="2" t="s">
         <v>9</v>
@@ -6093,10 +5878,10 @@
         <v>70</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E178" s="2" t="s">
         <v>9</v>
@@ -6115,82 +5900,83 @@
     </row>
     <row r="179" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="17">
-        <f t="shared" ref="A179:A183" si="4">ROW() - 1</f>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C179" s="5" t="s">
+      <c r="C179" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G179" s="3"/>
+      <c r="H179" s="3"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="3"/>
+      <c r="K179" s="3"/>
+      <c r="L179" s="3"/>
+      <c r="M179" s="3"/>
+      <c r="N179" s="3"/>
+    </row>
+    <row r="180" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A180" s="17">
+        <f t="shared" si="3"/>
+        <v>179</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C180" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D179" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E179" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F179" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G179" s="2"/>
-      <c r="H179" s="2"/>
-      <c r="I179" s="2"/>
-      <c r="J179" s="2"/>
-      <c r="K179" s="2"/>
-      <c r="L179" s="2"/>
-      <c r="M179" s="2"/>
-      <c r="N179" s="2"/>
-    </row>
-    <row r="180" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A180" s="19">
-        <f t="shared" si="4"/>
-        <v>179</v>
-      </c>
-      <c r="B180" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C180" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D180" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E180" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F180" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G180" s="13"/>
-      <c r="H180" s="13"/>
-      <c r="I180" s="13"/>
-      <c r="J180" s="13"/>
-      <c r="K180" s="13"/>
-      <c r="L180" s="13"/>
-      <c r="M180" s="13"/>
-      <c r="N180" s="13"/>
+      <c r="D180" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G180" s="2"/>
+      <c r="H180" s="2"/>
+      <c r="I180" s="2"/>
+      <c r="J180" s="2"/>
+      <c r="K180" s="2"/>
+      <c r="L180" s="2"/>
+      <c r="M180" s="2"/>
+      <c r="N180" s="2"/>
     </row>
     <row r="181" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C181" s="3" t="s">
+      <c r="C181" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D181" s="10" t="s">
-        <v>86</v>
+      <c r="D181" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E181" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G181" s="2"/>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
       <c r="J181" s="2"/>
@@ -6210,8 +5996,8 @@
       <c r="C182" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D182" s="3" t="s">
-        <v>71</v>
+      <c r="D182" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>9</v>
@@ -6230,7 +6016,7 @@
     </row>
     <row r="183" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A183:A187" si="4">ROW() - 1</f>
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
@@ -6240,10 +6026,10 @@
         <v>11</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
+      </c>
+      <c r="E183" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>10</v>
@@ -6258,29 +6044,54 @@
       <c r="N183" s="2"/>
     </row>
     <row r="184" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A184" s="17"/>
-      <c r="B184" s="2"/>
-      <c r="C184" s="5"/>
-      <c r="D184" s="3"/>
-      <c r="E184" s="2"/>
-      <c r="F184" s="2"/>
-      <c r="G184" s="2"/>
-      <c r="H184" s="2"/>
-      <c r="I184" s="2"/>
-      <c r="J184" s="2"/>
-      <c r="K184" s="2"/>
-      <c r="L184" s="2"/>
-      <c r="M184" s="2"/>
-      <c r="N184" s="2"/>
+      <c r="A184" s="19">
+        <f t="shared" si="4"/>
+        <v>183</v>
+      </c>
+      <c r="B184" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C184" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D184" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E184" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F184" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="13"/>
+      <c r="J184" s="13"/>
+      <c r="K184" s="13"/>
+      <c r="L184" s="13"/>
+      <c r="M184" s="13"/>
+      <c r="N184" s="13"/>
     </row>
     <row r="185" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A185" s="17"/>
-      <c r="B185" s="2"/>
-      <c r="C185" s="5"/>
-      <c r="D185" s="3"/>
-      <c r="E185" s="2"/>
-      <c r="F185" s="2"/>
-      <c r="G185" s="2"/>
+      <c r="A185" s="17">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
       <c r="J185" s="2"/>
@@ -6290,12 +6101,25 @@
       <c r="N185" s="2"/>
     </row>
     <row r="186" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A186" s="17"/>
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
-      <c r="D186" s="3"/>
-      <c r="E186" s="2"/>
-      <c r="F186" s="2"/>
+      <c r="A186" s="17">
+        <f t="shared" si="3"/>
+        <v>185</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G186" s="2"/>
       <c r="H186" s="2"/>
       <c r="I186" s="2"/>
@@ -6306,12 +6130,25 @@
       <c r="N186" s="2"/>
     </row>
     <row r="187" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A187" s="17"/>
-      <c r="B187" s="2"/>
-      <c r="C187" s="5"/>
-      <c r="D187" s="3"/>
-      <c r="E187" s="2"/>
-      <c r="F187" s="2"/>
+      <c r="A187" s="17">
+        <f t="shared" si="4"/>
+        <v>186</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C187" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G187" s="2"/>
       <c r="H187" s="2"/>
       <c r="I187" s="2"/>
@@ -6322,12 +6159,25 @@
       <c r="N187" s="2"/>
     </row>
     <row r="188" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A188" s="17"/>
-      <c r="B188" s="2"/>
-      <c r="C188" s="5"/>
-      <c r="D188" s="3"/>
-      <c r="E188" s="2"/>
-      <c r="F188" s="2"/>
+      <c r="A188" s="17">
+        <f t="shared" si="3"/>
+        <v>187</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G188" s="2"/>
       <c r="H188" s="2"/>
       <c r="I188" s="2"/>
@@ -6338,12 +6188,25 @@
       <c r="N188" s="2"/>
     </row>
     <row r="189" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A189" s="17"/>
-      <c r="B189" s="2"/>
-      <c r="C189" s="5"/>
-      <c r="D189" s="3"/>
-      <c r="E189" s="2"/>
-      <c r="F189" s="2"/>
+      <c r="A189" s="17">
+        <f t="shared" ref="A189:A191" si="5">ROW() - 1</f>
+        <v>188</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G189" s="2"/>
       <c r="H189" s="2"/>
       <c r="I189" s="2"/>
@@ -6354,12 +6217,25 @@
       <c r="N189" s="2"/>
     </row>
     <row r="190" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A190" s="17"/>
-      <c r="B190" s="2"/>
-      <c r="C190" s="5"/>
-      <c r="D190" s="3"/>
-      <c r="E190" s="2"/>
-      <c r="F190" s="2"/>
+      <c r="A190" s="17">
+        <f t="shared" si="5"/>
+        <v>189</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G190" s="2"/>
       <c r="H190" s="2"/>
       <c r="I190" s="2"/>
@@ -6370,12 +6246,25 @@
       <c r="N190" s="2"/>
     </row>
     <row r="191" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A191" s="17"/>
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
-      <c r="D191" s="2"/>
-      <c r="E191" s="2"/>
-      <c r="F191" s="2"/>
+      <c r="A191" s="17">
+        <f t="shared" si="5"/>
+        <v>190</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G191" s="2"/>
       <c r="H191" s="2"/>
       <c r="I191" s="2"/>
@@ -6388,8 +6277,8 @@
     <row r="192" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="17"/>
       <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
-      <c r="D192" s="2"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="3"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
@@ -6404,8 +6293,8 @@
     <row r="193" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="17"/>
       <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
-      <c r="D193" s="2"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="3"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
@@ -6420,8 +6309,8 @@
     <row r="194" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="17"/>
       <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
-      <c r="D194" s="2"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="3"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
@@ -19073,104 +18962,102 @@
       <c r="M984" s="2"/>
       <c r="N984" s="2"/>
     </row>
-    <row r="985" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="985" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A985" s="17"/>
       <c r="B985" s="2"/>
       <c r="C985" s="2"/>
       <c r="D985" s="2"/>
       <c r="E985" s="2"/>
       <c r="F985" s="2"/>
-    </row>
-    <row r="986" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G985" s="2"/>
+      <c r="H985" s="2"/>
+      <c r="I985" s="2"/>
+      <c r="J985" s="2"/>
+      <c r="K985" s="2"/>
+      <c r="L985" s="2"/>
+      <c r="M985" s="2"/>
+      <c r="N985" s="2"/>
+    </row>
+    <row r="986" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A986" s="17"/>
       <c r="B986" s="2"/>
       <c r="C986" s="2"/>
       <c r="D986" s="2"/>
       <c r="E986" s="2"/>
       <c r="F986" s="2"/>
+      <c r="G986" s="2"/>
+      <c r="H986" s="2"/>
+      <c r="I986" s="2"/>
+      <c r="J986" s="2"/>
+      <c r="K986" s="2"/>
+      <c r="L986" s="2"/>
+      <c r="M986" s="2"/>
+      <c r="N986" s="2"/>
+    </row>
+    <row r="987" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A987" s="17"/>
+      <c r="B987" s="2"/>
+      <c r="C987" s="2"/>
+      <c r="D987" s="2"/>
+      <c r="E987" s="2"/>
+      <c r="F987" s="2"/>
+      <c r="G987" s="2"/>
+      <c r="H987" s="2"/>
+      <c r="I987" s="2"/>
+      <c r="J987" s="2"/>
+      <c r="K987" s="2"/>
+      <c r="L987" s="2"/>
+      <c r="M987" s="2"/>
+      <c r="N987" s="2"/>
+    </row>
+    <row r="988" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A988" s="17"/>
+      <c r="B988" s="2"/>
+      <c r="C988" s="2"/>
+      <c r="D988" s="2"/>
+      <c r="E988" s="2"/>
+      <c r="F988" s="2"/>
+      <c r="G988" s="2"/>
+      <c r="H988" s="2"/>
+      <c r="I988" s="2"/>
+      <c r="J988" s="2"/>
+      <c r="K988" s="2"/>
+      <c r="L988" s="2"/>
+      <c r="M988" s="2"/>
+      <c r="N988" s="2"/>
+    </row>
+    <row r="989" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A989" s="17"/>
+      <c r="B989" s="2"/>
+      <c r="C989" s="2"/>
+      <c r="D989" s="2"/>
+      <c r="E989" s="2"/>
+      <c r="F989" s="2"/>
+    </row>
+    <row r="990" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A990" s="17"/>
+      <c r="B990" s="2"/>
+      <c r="C990" s="2"/>
+      <c r="D990" s="2"/>
+      <c r="E990" s="2"/>
+      <c r="F990" s="2"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A950"/>
+      <autoFilter ref="A1:A950" xr:uid="{E506BC01-76C4-4025-8B5F-5582097F295F}"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F174 F1:F44 F176:F986 F139:F172 F48:F136">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Read">
+  <conditionalFormatting sqref="F1:F990">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH(("No"),(F1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Write">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Write">
       <formula>NOT(ISERROR(SEARCH(("Write"),(F1))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F173">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F173))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F173))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F173))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F175">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F175))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F175))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F175))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F137:F138">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F137))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F137))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F137))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F45))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F45))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F45))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F46))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F46))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F46))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Read">
-      <formula>NOT(ISERROR(SEARCH(("Read"),(F47))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH(("No"),(F47))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Write">
-      <formula>NOT(ISERROR(SEARCH(("Write"),(F47))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19178,35 +19065,35 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B36 B136:B179 B182:B1048576 B94:B134 B38:B92</xm:sqref>
+          <xm:sqref>B1:B36 B38:B92 B136:B183 B94:B134 B186:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$B$2:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E35 E136:E179 E182:E1048576 E94:E134 E38:E90</xm:sqref>
+          <xm:sqref>E1:E35 E38:E90 E136:E183 E94:E134 E186:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$B$3:$B$77</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D35 D182:D1048576 D94:D134 D137:D179 D38:D90</xm:sqref>
+          <xm:sqref>D1:D35 D137:D183 D94:D134 D38:D90 D186:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F35 F136:F179 F182:F1048576 F94:F134 F38:F90</xm:sqref>
+          <xm:sqref>F1:F35 F38:F90 F136:F183 F94:F134 F186:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ScreenIds!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C35 C136:C179 C92 C182:C1048576 C94:C134 C38:C90</xm:sqref>
+          <xm:sqref>C1:C35 C38:C90 C92 C136:C183 C94:C134 C186:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19215,7 +19102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -19658,7 +19545,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B4:B73">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B73">
     <sortCondition ref="B3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>